<commit_message>
MASC runs!, Curious preliminary results, need more data cleaning
</commit_message>
<xml_diff>
--- a/data/umweltbundesamt/umweltzonen.xlsx
+++ b/data/umweltbundesamt/umweltzonen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aavil\OneDrive\Documentos\A - Estudios\LSE_ASDS\Project\Capstone-Project\data\umweltbundesamt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F41A05A-EE03-4FDD-8EC8-6C06230A3FF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B7A1F7-87D6-4F33-96BF-81C0909161E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -386,9 +386,6 @@
     <t>https://web.archive.org/web/20070325091507/http://www.rp.baden-wuerttemberg.de/servlet/PB/show/1159769/rpf-ref54.1-lrp.pdf</t>
   </si>
   <si>
-    <t>01.03.2017</t>
-  </si>
-  <si>
     <t xml:space="preserve">I am a student who wants to look at the positive/negative effects of german Low Emissions Zones and their pollution reduction in economic output and labor productivity. For that I need to know the announcment date (not application)  of each umweltzone. I have extensively searched on your current webpage and platform but there is no such data. </t>
   </si>
   <si>
@@ -489,6 +486,9 @@
   </si>
   <si>
     <t>https://www.umwelt.niedersachsen.de/startseite/themen/luftqualitat/luftschadstoffberechnungen_amp_luftreinhalteplane/luftreinhalteplane/lrp_hannover/luftreinhalteplan-fuer-hannover-8921.html</t>
+  </si>
+  <si>
+    <t>01.03.2006</t>
   </si>
 </sst>
 </file>
@@ -893,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -931,7 +931,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -976,13 +976,13 @@
         <v>9</v>
       </c>
       <c r="H3" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1059,13 +1059,13 @@
         <v>20</v>
       </c>
       <c r="H6" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1099,7 +1099,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -1114,10 +1114,10 @@
         <v>26</v>
       </c>
       <c r="H8" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1246,7 +1246,7 @@
         <v>38</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
@@ -1284,7 +1284,7 @@
         <v>42</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>119</v>
@@ -1360,10 +1360,10 @@
         <v>20</v>
       </c>
       <c r="H18" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="I18" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1607,13 +1607,13 @@
         <v>34</v>
       </c>
       <c r="H28" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="I28" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="J28" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1624,7 +1624,7 @@
         <v>61</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
@@ -1672,7 +1672,7 @@
         <v>65</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D31" t="s">
         <v>6</v>
@@ -1856,13 +1856,13 @@
         <v>31</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I38" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="J38" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2136,7 +2136,7 @@
         <v>98</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D50" t="s">
         <v>6</v>
@@ -2301,7 +2301,7 @@
         <v>107</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D57" t="s">
         <v>6</v>
@@ -2324,7 +2324,7 @@
         <v>108</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D58" t="s">
         <v>6</v>
@@ -2461,48 +2461,48 @@
     </row>
     <row r="4" spans="2:3">
       <c r="B4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="2:3">
       <c r="B9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="2:3">
       <c r="B11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="2:3">
       <c r="B13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish of day some good results on MASC
Delete Spain, Portugal and Greece was VERY good
</commit_message>
<xml_diff>
--- a/data/umweltbundesamt/umweltzonen.xlsx
+++ b/data/umweltbundesamt/umweltzonen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aavil\OneDrive\Documentos\A - Estudios\LSE_ASDS\Project\Capstone-Project\data\umweltbundesamt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B7A1F7-87D6-4F33-96BF-81C0909161E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B117CC68-4751-4E61-9CAC-56A907991ABA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="160">
   <si>
     <t xml:space="preserve">Das Umweltbundesamt stellt die von den Ländern und Kommunen gemeldeten Informationen über Umweltzonen in dieser Übersicht für das gesamte Gebiet der Bundesrepublik zusammen. Für die Aktualität, Vollständigkeit und Richtigkeit der Angaben sind die jeweiligen Kommunen verantwortlich. </t>
   </si>
@@ -489,6 +489,21 @@
   </si>
   <si>
     <t>01.03.2006</t>
+  </si>
+  <si>
+    <t>10.10.2012</t>
+  </si>
+  <si>
+    <t>https://www.erfurt.de/ef/de/leben/verkehr/mobil/auto/umweltzone/index.html</t>
+  </si>
+  <si>
+    <t>09.12.2008</t>
+  </si>
+  <si>
+    <t>https://www.osnabrueck.de/umweltzone/</t>
+  </si>
+  <si>
+    <t>https://www.stadt-muenster.de/umwelt/immissionsschutz/luft/umweltzone.html</t>
   </si>
 </sst>
 </file>
@@ -571,11 +586,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -893,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="C26" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -910,15 +925,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
       <c r="I1" s="4" t="s">
         <v>117</v>
       </c>
@@ -1214,6 +1229,12 @@
       <c r="G12" t="s">
         <v>31</v>
       </c>
+      <c r="H12" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
@@ -1805,7 +1826,6 @@
       <c r="G36" t="s">
         <v>23</v>
       </c>
-      <c r="I36" s="2"/>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
@@ -1855,7 +1875,7 @@
       <c r="G38" t="s">
         <v>31</v>
       </c>
-      <c r="H38" s="14" t="s">
+      <c r="H38" s="12" t="s">
         <v>146</v>
       </c>
       <c r="I38" s="4" t="s">
@@ -1887,7 +1907,12 @@
       <c r="G39" t="s">
         <v>78</v>
       </c>
-      <c r="I39" s="2"/>
+      <c r="H39" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
@@ -1983,6 +2008,12 @@
       </c>
       <c r="G43" t="s">
         <v>89</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2416,9 +2447,12 @@
     <hyperlink ref="J28" r:id="rId17" xr:uid="{2749FEE2-BF00-4274-B7DF-5EA7EB307E53}"/>
     <hyperlink ref="I8" r:id="rId18" xr:uid="{7D56F90E-1E4B-4482-81F9-FCD49BE68261}"/>
     <hyperlink ref="I18" r:id="rId19" xr:uid="{3C013743-470B-4F05-B9C1-3582B2F51821}"/>
+    <hyperlink ref="I12" r:id="rId20" xr:uid="{4014BD27-873D-44F8-B7FB-9D13C1798518}"/>
+    <hyperlink ref="I43" r:id="rId21" xr:uid="{614EB40E-8487-40DF-AEC5-FD79790069F6}"/>
+    <hyperlink ref="I39" r:id="rId22" xr:uid="{99F92922-FCBB-4BE6-820A-765A34625186}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId23"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Abandon MASC + Center in Gsynth
Masc was useless if the pollution data was not good enough

Gsynth woks fairly good.

Doubts about confounders for unemployment
</commit_message>
<xml_diff>
--- a/data/umweltbundesamt/umweltzonen.xlsx
+++ b/data/umweltbundesamt/umweltzonen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aavil\OneDrive\Documentos\A - Estudios\LSE_ASDS\Project\Capstone-Project\data\umweltbundesamt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B117CC68-4751-4E61-9CAC-56A907991ABA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B072F82-FBDF-4714-827B-3BDA86041B6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="163">
   <si>
     <t xml:space="preserve">Das Umweltbundesamt stellt die von den Ländern und Kommunen gemeldeten Informationen über Umweltzonen in dieser Übersicht für das gesamte Gebiet der Bundesrepublik zusammen. Für die Aktualität, Vollständigkeit und Richtigkeit der Angaben sind die jeweiligen Kommunen verantwortlich. </t>
   </si>
@@ -504,6 +504,15 @@
   </si>
   <si>
     <t>https://www.stadt-muenster.de/umwelt/immissionsschutz/luft/umweltzone.html</t>
+  </si>
+  <si>
+    <t>really 11.2014</t>
+  </si>
+  <si>
+    <t>https://www.offenbach.de/leben-in-of/umwelt-klimaschutz/Luft_Laerm/Luftreinhaltung/testartikel-umweltzone.php</t>
+  </si>
+  <si>
+    <t>01.11.2014</t>
   </si>
 </sst>
 </file>
@@ -573,7 +582,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -591,6 +600,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -908,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C26" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1985,7 +1995,15 @@
       <c r="G42" t="s">
         <v>78</v>
       </c>
-      <c r="I42" s="2"/>
+      <c r="H42" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
@@ -2450,9 +2468,10 @@
     <hyperlink ref="I12" r:id="rId20" xr:uid="{4014BD27-873D-44F8-B7FB-9D13C1798518}"/>
     <hyperlink ref="I43" r:id="rId21" xr:uid="{614EB40E-8487-40DF-AEC5-FD79790069F6}"/>
     <hyperlink ref="I39" r:id="rId22" xr:uid="{99F92922-FCBB-4BE6-820A-765A34625186}"/>
+    <hyperlink ref="J42" r:id="rId23" xr:uid="{1DDA0C60-77E5-4EBD-AD0B-DCBA4D6A2DF5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Data refresher with new dates
</commit_message>
<xml_diff>
--- a/data/umweltbundesamt/umweltzonen.xlsx
+++ b/data/umweltbundesamt/umweltzonen.xlsx
@@ -8,23 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aavil\OneDrive\Documentos\A - Estudios\LSE_ASDS\Project\Capstone-Project\data\umweltbundesamt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B072F82-FBDF-4714-827B-3BDA86041B6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2845596D-02A7-4D16-B510-5B696812B98C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sources of info" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$I$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet2!$A$2:$I$60</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="188">
   <si>
     <t xml:space="preserve">Das Umweltbundesamt stellt die von den Ländern und Kommunen gemeldeten Informationen über Umweltzonen in dieser Übersicht für das gesamte Gebiet der Bundesrepublik zusammen. Für die Aktualität, Vollständigkeit und Richtigkeit der Angaben sind die jeweiligen Kommunen verantwortlich. </t>
   </si>
@@ -374,18 +376,12 @@
     <t>06.01.2017</t>
   </si>
   <si>
-    <t>https://www.schwarzwald-netz.com/168/Schwarzwald-Anreise/Umwelt-Zonen-und-Schadstoffplaketten-Schwarzwald.html</t>
-  </si>
-  <si>
     <t>https://web.archive.org/web/20070607195753/http://www.env-it.de/luftdaten/download/public/html/Umweltzonen/index.htm</t>
   </si>
   <si>
     <t>https://web.archive.org/web/20070607174634/http://www.umweltbundesamt.de/uba-info-presse/2007/pd07-037.htm</t>
   </si>
   <si>
-    <t>https://web.archive.org/web/20070325091507/http://www.rp.baden-wuerttemberg.de/servlet/PB/show/1159769/rpf-ref54.1-lrp.pdf</t>
-  </si>
-  <si>
     <t xml:space="preserve">I am a student who wants to look at the positive/negative effects of german Low Emissions Zones and their pollution reduction in economic output and labor productivity. For that I need to know the announcment date (not application)  of each umweltzone. I have extensively searched on your current webpage and platform but there is no such data. </t>
   </si>
   <si>
@@ -410,15 +406,6 @@
     <t>DW</t>
   </si>
   <si>
-    <t>20.03.2007</t>
-  </si>
-  <si>
-    <t>https://www.berlin.de/senuvk/umwelt/luftqualitaet/de/luftreinhalteplan/download/2005/anpassung_aktionsplan_umweltzone.pdf</t>
-  </si>
-  <si>
-    <t>https://www.berlin.de/senuvk/umwelt/luftqualitaet/de/luftreinhalteplan/doku_lrp_2005_2010.shtml</t>
-  </si>
-  <si>
     <t>Good:</t>
   </si>
   <si>
@@ -449,70 +436,160 @@
     <t>Urbach (Baden-Württemberg)</t>
   </si>
   <si>
-    <t>20.10.2015</t>
-  </si>
-  <si>
-    <t>http://www.aachen.de/DE/stadt_buerger/umwelt/luft-stadtklima/luftreinhalteplan_umweltzone/umweltzone/pressemitteilungen/presseinfo_2015_01_20.html</t>
-  </si>
-  <si>
-    <t>http://www.aachen.de/DE/stadt_buerger/umwelt/luft-stadtklima/luftreinhalteplan_umweltzone/umweltzone/pressemitteilungen/index.html</t>
-  </si>
-  <si>
-    <t>https://www.muenchen.de/rathaus/dam/jcr:9ea7e64e-d963-4208-8459-1ce7ca763514/3.%20Fortschreibung%20des%20Luftreinhalteplans.pdf</t>
-  </si>
-  <si>
-    <t>https://www.muenchen.de/rathaus/Stadtverwaltung/Referat-fuer-Gesundheit-und-Umwelt/Luft_und_Strahlung/Luftreinhalteplan.html#2-fortschreibung-des-luftreinhalteplans_13</t>
-  </si>
-  <si>
-    <t>21.08.2008</t>
-  </si>
-  <si>
-    <t>18.12.2009</t>
-  </si>
-  <si>
-    <t>https://static.leipzig.de/fileadmin/mediendatenbank/leipzig-de/Stadt/02.3_Dez3_Umwelt_Ordnung_Sport/36_Amt_fuer_Umweltschutz/Luft_und_Laerm/Luftreinhaltung/Luftreinhalteplan/Luftreinhalteplan_2009.pdf</t>
-  </si>
-  <si>
-    <t>https://www.leipzig.de/umwelt-und-verkehr/luft-und-laerm/luftreinhaltung/luftreinhalteplan-der-stadt-leipzig/</t>
-  </si>
-  <si>
-    <t>01.08.2006</t>
-  </si>
-  <si>
-    <t>https://www.bauumwelt.bremen.de/umwelt/luft/umweltzone_bremen-24570</t>
-  </si>
-  <si>
-    <t>01.07.2007</t>
-  </si>
-  <si>
-    <t>https://www.umwelt.niedersachsen.de/startseite/themen/luftqualitat/luftschadstoffberechnungen_amp_luftreinhalteplane/luftreinhalteplane/lrp_hannover/luftreinhalteplan-fuer-hannover-8921.html</t>
-  </si>
-  <si>
-    <t>01.03.2006</t>
-  </si>
-  <si>
-    <t>10.10.2012</t>
-  </si>
-  <si>
-    <t>https://www.erfurt.de/ef/de/leben/verkehr/mobil/auto/umweltzone/index.html</t>
-  </si>
-  <si>
-    <t>09.12.2008</t>
-  </si>
-  <si>
-    <t>https://www.osnabrueck.de/umweltzone/</t>
-  </si>
-  <si>
-    <t>https://www.stadt-muenster.de/umwelt/immissionsschutz/luft/umweltzone.html</t>
-  </si>
-  <si>
-    <t>really 11.2014</t>
-  </si>
-  <si>
-    <t>https://www.offenbach.de/leben-in-of/umwelt-klimaschutz/Luft_Laerm/Luftreinhaltung/testartikel-umweltzone.php</t>
-  </si>
-  <si>
-    <t>01.11.2014</t>
+    <t xml:space="preserve">Das Umweltbundesamt stellt die von den Ländern und Kommunen gemeldeten Informationen über Umweltzonen in dieser Übersicht für das gesamte Gebiet der Bundesrepublik zusammen/ Für die Aktualität, Vollständigkeit und Richtigkeit der Angaben sind die jeweiligen Kommunen verantwortlich/ </t>
+  </si>
+  <si>
+    <t>https://web/archive/org/web/20070607195753/http://www/env-it/de/luftdaten/download/public/html/Umweltzonen/index/htm</t>
+  </si>
+  <si>
+    <t>https://www/berlin/de/senuvk/umwelt/luftqualitaet/de/luftreinhalteplan/download/2005/anpassung_aktionsplan_umweltzone/pdf</t>
+  </si>
+  <si>
+    <t>http://www/aachen/de/DE/stadt_buerger/umwelt/luft-stadtklima/luftreinhalteplan_umweltzone/umweltzone/pressemitteilungen/index/html</t>
+  </si>
+  <si>
+    <t>https://www/umwelt/niedersachsen/de/startseite/themen/luftqualitat/luftschadstoffberechnungen_amp_luftreinhalteplane/luftreinhalteplane/lrp_hannover/luftreinhalteplan-fuer-hannover-8921/html</t>
+  </si>
+  <si>
+    <t>https://www/schwarzwald-netz/com/168/Schwarzwald-Anreise/Umwelt-Zonen-und-Schadstoffplaketten-Schwarzwald/html</t>
+  </si>
+  <si>
+    <t>https://www/bauumwelt/bremen/de/umwelt/luft/umweltzone_bremen-24570</t>
+  </si>
+  <si>
+    <t>https://www/berlin/de/senuvk/umwelt/luftqualitaet/de/luftreinhalteplan/doku_lrp_2005_2010/shtml</t>
+  </si>
+  <si>
+    <t>https://web/archive/org/web/20070325091507/http://www/rp/baden-wuerttemberg/de/servlet/PB/show/1159769/rpf-ref54/1-lrp/pdf</t>
+  </si>
+  <si>
+    <t>Ruhrgebiet(Bochum, Bottrop, Castrop-Rauxel, ///</t>
+  </si>
+  <si>
+    <t>Ludwigsburg und Umgebung(Asperg, ///</t>
+  </si>
+  <si>
+    <t>really 11/2014</t>
+  </si>
+  <si>
+    <t>http://www/aachen/de/DE/stadt_buerger/umwelt/luft-stadtklima/luftreinhalteplan_umweltzone/umweltzone/pressemitteilungen/presseinfo_2015_01_20/html</t>
+  </si>
+  <si>
+    <t>https://static/leipzig/de/fileadmin/mediendatenbank/leipzig-de/Stadt/02/3_Dez3_Umwelt_Ordnung_Sport/36_Amt_fuer_Umweltschutz/Luft_und_Laerm/Luftreinhaltung/Luftreinhalteplan/Luftreinhalteplan_2009/pdf</t>
+  </si>
+  <si>
+    <t>https://www/offenbach/de/leben-in-of/umwelt-klimaschutz/Luft_Laerm/Luftreinhaltung/testartikel-umweltzone/php</t>
+  </si>
+  <si>
+    <t>Frankfurt a/M/</t>
+  </si>
+  <si>
+    <t>https://www/muenchen/de/rathaus/dam/jcr:9ea7e64e-d963-4208-8459-1ce7ca763514/3/%20Fortschreibung%20des%20Luftreinhalteplans/pdf</t>
+  </si>
+  <si>
+    <t>https://www/erfurt/de/ef/de/leben/verkehr/mobil/auto/umweltzone/index/html</t>
+  </si>
+  <si>
+    <t>Leonberg / Hemmingen und Umgebung(Ditzingen, ///</t>
+  </si>
+  <si>
+    <t>https://www/osnabrueck/de/umweltzone/</t>
+  </si>
+  <si>
+    <t>pdf at the end</t>
+  </si>
+  <si>
+    <t>https://www.eschweiler.de/buergerservice/leistungen/NRW:entry:609-VLR/umweltzone/</t>
+  </si>
+  <si>
+    <t>https://www.marburg.de/portal/seiten/luft-reinhaltung-900000917-23001.html?rubrik=900000045</t>
+  </si>
+  <si>
+    <t>https://www.darmstadt.de/fileadmin/PDF-Rubriken/Leben_in_Darmstadt/umwelt/umweltzone.pdf</t>
+  </si>
+  <si>
+    <t>https://www.siegen.de/fileadmin/cms/pdf/Umwelt/Luftreinhaltung/LuftreinhalteplanSiegen2014.pdf</t>
+  </si>
+  <si>
+    <t>https://rp.baden-wuerttemberg.de/rps/Abt5/Ref541/Luftreinhalteplan/541_s_luft_leo_fortschr_Immissionsgut_Lohmeyer.pdf</t>
+  </si>
+  <si>
+    <t>https://rp.baden-wuerttemberg.de/rpf/Abt5/Ref541/Luftreinhaltung/Seiten/Region-Schramberg.aspx</t>
+  </si>
+  <si>
+    <t>https://rp.baden-wuerttemberg.de/rps/Abt5/Ref541/Luftreinhalteplan/541_s_luft_wendl_stufe3.pdf</t>
+  </si>
+  <si>
+    <t>https://lfu.rlp.de/fileadmin/lfu/Downloads/Luftreinhaltung/Luftreinhaltenplan_Mainz_17012012Internetversion.pdf</t>
+  </si>
+  <si>
+    <t>https://www.hlnug.de/fileadmin/dokumente/luft/luftreinhalteplaene/2012/1_Fortschreibung_LRP_Ballungsraum_Rhein-Main_Teilplan_Wiesbaden.pdf</t>
+  </si>
+  <si>
+    <t>https://www.langenfeld.de/city_info/webaccessibility/index.cfm?item_id=853021&amp;modul_id=5&amp;record_id=84153</t>
+  </si>
+  <si>
+    <t>https://rp.baden-wuerttemberg.de/rps/Abt5/Ref541/Luftreinhalteplan/541_s_luft_lb_massnahmen_12.pdf</t>
+  </si>
+  <si>
+    <t>https://www.moenchengladbach.de/de/rathaus/buergerinfo-a-z/planen-bauen-mobilitaet-umwelt-dezernat-vi/fachbereich-umwelt-64/landschaft-luftklima-immissionen/luftqualitaet-in-moenchengladbach/</t>
+  </si>
+  <si>
+    <t>https://remscheid.de/leben/umwelt-und-natur/umweltschutz/146380100000099860.php</t>
+  </si>
+  <si>
+    <t>https://www.hagen.de/web/media/files/fb/fb_69/luftreinhalteplaene/umweltzone/Allgemeinverfuegung_Umweltzone_HAGEN.pdf</t>
+  </si>
+  <si>
+    <t>https://rp.baden-wuerttemberg.de/rps/Abt5/Ref541/Luftreinhalteplan/541_s_luft_hdh_massnahmenb.pdf</t>
+  </si>
+  <si>
+    <t>https://www.bochum.de/C125830C0042AB74/vwContentByKey/W2BMZEU9999BOCMDE/$File/luftreinhalteplan_Ruhrgebiet_ost.pdf</t>
+  </si>
+  <si>
+    <t>? Month?</t>
+  </si>
+  <si>
+    <t>https://rp.baden-wuerttemberg.de/rps/Abt5/Ref541/Luftreinhalteplan/541_s_luft_urbach_Massnahmenb.pdf</t>
+  </si>
+  <si>
+    <t>Search for environmental plan</t>
+  </si>
+  <si>
+    <t>http://www.halle.de/de/Verwaltung/Umwelt/Luft-Laerm-Elektrosmog/Luft/Umweltzone/</t>
+  </si>
+  <si>
+    <t>12. April 2011</t>
+  </si>
+  <si>
+    <t>https://www.magdeburg.de/PDF/Luftreinhalteplan_Umweltzone.PDF?ObjSvrID=698&amp;ObjID=12588&amp;ObjLa=1&amp;Ext=PDF&amp;WTR=1&amp;_ts=1553846048</t>
+  </si>
+  <si>
+    <t>(draft)</t>
+  </si>
+  <si>
+    <t>https://www.dinslaken.de/de/wirtschaft-wohnen/luftreinhalteplanung/</t>
+  </si>
+  <si>
+    <t>https://www.bezreg-muenster.de/de/umwelt_und_natur/umweltzonen_und_luftreinhalteplaene/index.html</t>
+  </si>
+  <si>
+    <t>http://www.brd.nrw.de/Umweltschutz_Luftreinhaltung/pdf/2019_10_31_Endfassung_LRP_Krefeld.pdf</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>https://www.neuss.de/leben/umwelt-und-gruen/umweltzone/luftreinhalteplan-neuss</t>
+  </si>
+  <si>
+    <t>https://www.bonn.de/themen-entdecken/umwelt-natur/luftreinhalteplan.php</t>
+  </si>
+  <si>
+    <t>https://rp.baden-wuerttemberg.de/rpk/Abt5/Ref541/Seiten/Luftreinhalteplaene.aspx</t>
+  </si>
+  <si>
+    <t>https://rp.baden-wuerttemberg.de/rpk/Abt5/Ref541/Luftreinhalteplan/rpk54.1_lrp_pfinz__entwurf_internet.pdf</t>
   </si>
 </sst>
 </file>
@@ -558,13 +635,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -582,25 +659,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -918,34 +996,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="25.6328125" customWidth="1"/>
-    <col min="2" max="2" width="54" customWidth="1"/>
-    <col min="3" max="3" width="54" style="11" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" style="7" customWidth="1"/>
     <col min="4" max="4" width="9.453125" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" style="5" customWidth="1"/>
     <col min="6" max="6" width="13.453125" customWidth="1"/>
     <col min="7" max="7" width="16.1796875" customWidth="1"/>
     <col min="8" max="8" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="I1" s="4" t="s">
-        <v>117</v>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="I1" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -956,12 +1034,12 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -976,7 +1054,7 @@
       <c r="I2" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J2" s="11"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
@@ -985,13 +1063,13 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
@@ -1000,14 +1078,14 @@
       <c r="G3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>143</v>
+      <c r="H3" s="11">
+        <v>42297</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1017,13 +1095,13 @@
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F4" t="s">
@@ -1032,10 +1110,11 @@
       <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="4" t="s">
-        <v>116</v>
-      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
@@ -1044,13 +1123,13 @@
       <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F5" t="s">
@@ -1059,7 +1138,9 @@
       <c r="G5" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="2"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
@@ -1068,13 +1149,13 @@
       <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F6" t="s">
@@ -1083,14 +1164,14 @@
       <c r="G6" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>130</v>
+      <c r="H6" s="11">
+        <v>39161</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1100,13 +1181,13 @@
       <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F7" t="s">
@@ -1114,6 +1195,15 @@
       </c>
       <c r="G7" t="s">
         <v>23</v>
+      </c>
+      <c r="H7" s="5">
+        <v>40087</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1123,13 +1213,13 @@
       <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>139</v>
+      <c r="C8" s="7" t="s">
+        <v>134</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F8" t="s">
@@ -1138,12 +1228,13 @@
       <c r="G8" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>151</v>
-      </c>
+      <c r="H8" s="12">
+        <v>38930</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
@@ -1152,13 +1243,13 @@
       <c r="B9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>29</v>
       </c>
       <c r="F9" t="s">
@@ -1167,7 +1258,13 @@
       <c r="G9" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="2"/>
+      <c r="H9" s="14">
+        <v>42010</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
@@ -1176,13 +1273,13 @@
       <c r="B10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="7" t="s">
         <v>30</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F10" t="s">
@@ -1191,7 +1288,13 @@
       <c r="G10" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="2"/>
+      <c r="H10" s="13">
+        <v>40459</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
@@ -1200,13 +1303,13 @@
       <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F11" t="s">
@@ -1215,7 +1318,9 @@
       <c r="G11" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="2"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
@@ -1224,13 +1329,13 @@
       <c r="B12" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F12" t="s">
@@ -1239,12 +1344,13 @@
       <c r="G12" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>156</v>
-      </c>
+      <c r="H12" s="11">
+        <v>41192</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
@@ -1253,13 +1359,13 @@
       <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="7" t="s">
         <v>37</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F13" t="s">
@@ -1268,6 +1374,13 @@
       <c r="G13" t="s">
         <v>14</v>
       </c>
+      <c r="H13" s="13">
+        <v>42461</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
@@ -1276,13 +1389,13 @@
       <c r="B14" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>134</v>
+      <c r="C14" s="7" t="s">
+        <v>129</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>39</v>
       </c>
       <c r="F14" t="s">
@@ -1291,6 +1404,9 @@
       <c r="G14" t="s">
         <v>40</v>
       </c>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
@@ -1299,13 +1415,13 @@
       <c r="B15" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F15" t="s">
@@ -1314,12 +1430,13 @@
       <c r="G15" t="s">
         <v>42</v>
       </c>
-      <c r="H15" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>119</v>
-      </c>
+      <c r="H15" s="12">
+        <v>38777</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
@@ -1328,13 +1445,13 @@
       <c r="B16" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="7" t="s">
         <v>43</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F16" t="s">
@@ -1343,7 +1460,13 @@
       <c r="G16" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="2"/>
+      <c r="H16" s="14">
+        <v>40856</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
@@ -1352,13 +1475,13 @@
       <c r="B17" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="7" t="s">
         <v>45</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>46</v>
       </c>
       <c r="F17" t="s">
@@ -1367,6 +1490,13 @@
       <c r="G17" t="s">
         <v>42</v>
       </c>
+      <c r="H17" s="13">
+        <v>40664</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
@@ -1375,13 +1505,13 @@
       <c r="B18" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="7" t="s">
         <v>48</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>19</v>
       </c>
       <c r="F18" t="s">
@@ -1390,12 +1520,13 @@
       <c r="G18" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>153</v>
-      </c>
+      <c r="H18" s="12">
+        <v>39264</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="J18" s="8"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
@@ -1404,13 +1535,13 @@
       <c r="B19" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="7" t="s">
         <v>49</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F19" t="s">
@@ -1419,6 +1550,13 @@
       <c r="G19" t="s">
         <v>42</v>
       </c>
+      <c r="H19" s="13">
+        <v>38758</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="J19" s="8"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
@@ -1427,13 +1565,13 @@
       <c r="B20" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="7" t="s">
         <v>50</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F20" t="s">
@@ -1442,7 +1580,13 @@
       <c r="G20" t="s">
         <v>42</v>
       </c>
-      <c r="I20" s="2"/>
+      <c r="H20" s="13">
+        <v>40848</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
@@ -1451,13 +1595,13 @@
       <c r="B21" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F21" t="s">
@@ -1466,6 +1610,9 @@
       <c r="G21" t="s">
         <v>42</v>
       </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
@@ -1474,13 +1621,13 @@
       <c r="B22" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F22" t="s">
@@ -1489,9 +1636,11 @@
       <c r="G22" t="s">
         <v>42</v>
       </c>
-      <c r="I22" t="s">
-        <v>116</v>
-      </c>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="J22" s="8"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
@@ -1500,13 +1649,13 @@
       <c r="B23" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="7" t="s">
         <v>53</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="5" t="s">
         <v>54</v>
       </c>
       <c r="F23" t="s">
@@ -1515,6 +1664,9 @@
       <c r="G23" t="s">
         <v>42</v>
       </c>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
@@ -1523,13 +1675,13 @@
       <c r="B24" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="7" t="s">
         <v>55</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F24" t="s">
@@ -1538,9 +1690,11 @@
       <c r="G24" t="s">
         <v>42</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>116</v>
-      </c>
+      <c r="H24" s="8"/>
+      <c r="I24" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J24" s="8"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
@@ -1549,13 +1703,13 @@
       <c r="B25" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="7" t="s">
         <v>57</v>
       </c>
       <c r="D25" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="5" t="s">
         <v>19</v>
       </c>
       <c r="F25" t="s">
@@ -1564,8 +1718,12 @@
       <c r="G25" t="s">
         <v>23</v>
       </c>
-      <c r="I25" s="4" t="s">
-        <v>116</v>
+      <c r="H25" s="8"/>
+      <c r="I25" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1575,13 +1733,13 @@
       <c r="B26" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="7" t="s">
         <v>56</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F26" t="s">
@@ -1590,7 +1748,13 @@
       <c r="G26" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="2"/>
+      <c r="H26" s="5">
+        <v>40452</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="J26" s="8"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
@@ -1599,13 +1763,13 @@
       <c r="B27" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="7" t="s">
         <v>58</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F27" t="s">
@@ -1613,6 +1777,15 @@
       </c>
       <c r="G27" t="s">
         <v>23</v>
+      </c>
+      <c r="H27" s="13">
+        <v>41153</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1622,13 +1795,13 @@
       <c r="B28" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="7" t="s">
         <v>60</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="5" t="s">
         <v>34</v>
       </c>
       <c r="F28" t="s">
@@ -1637,14 +1810,14 @@
       <c r="G28" t="s">
         <v>34</v>
       </c>
-      <c r="H28" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="J28" s="4" t="s">
+      <c r="H28" s="12">
+        <v>40165</v>
+      </c>
+      <c r="I28" s="3" t="s">
         <v>149</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1654,13 +1827,13 @@
       <c r="B29" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>136</v>
+      <c r="C29" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="5" t="s">
         <v>62</v>
       </c>
       <c r="F29" t="s">
@@ -1669,8 +1842,15 @@
       <c r="G29" t="s">
         <v>62</v>
       </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
+      <c r="H29" s="13">
+        <v>40695</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
@@ -1679,13 +1859,13 @@
       <c r="B30" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="7" t="s">
         <v>63</v>
       </c>
       <c r="D30" t="s">
         <v>6</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="5" t="s">
         <v>64</v>
       </c>
       <c r="F30" t="s">
@@ -1694,6 +1874,9 @@
       <c r="G30" t="s">
         <v>64</v>
       </c>
+      <c r="H30" s="15"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
@@ -1702,13 +1885,13 @@
       <c r="B31" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>137</v>
+      <c r="C31" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="D31" t="s">
         <v>6</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F31" t="s">
@@ -1717,6 +1900,13 @@
       <c r="G31" t="s">
         <v>42</v>
       </c>
+      <c r="H31" s="13">
+        <v>41183</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="J31" s="8"/>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
@@ -1725,13 +1915,13 @@
       <c r="B32" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="7" t="s">
         <v>66</v>
       </c>
       <c r="D32" t="s">
         <v>6</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="5" t="s">
         <v>46</v>
       </c>
       <c r="F32" t="s">
@@ -1739,6 +1929,15 @@
       </c>
       <c r="G32" t="s">
         <v>42</v>
+      </c>
+      <c r="H32" s="13">
+        <v>40645</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1748,13 +1947,13 @@
       <c r="B33" t="s">
         <v>68</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="7" t="s">
         <v>68</v>
       </c>
       <c r="D33" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E33" s="5" t="s">
         <v>69</v>
       </c>
       <c r="F33" t="s">
@@ -1763,7 +1962,13 @@
       <c r="G33" t="s">
         <v>69</v>
       </c>
-      <c r="I33" s="2"/>
+      <c r="H33" s="13">
+        <v>40264</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="J33" s="8"/>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
@@ -1772,13 +1977,13 @@
       <c r="B34" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
       <c r="D34" t="s">
         <v>6</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="5" t="s">
         <v>54</v>
       </c>
       <c r="F34" t="s">
@@ -1787,9 +1992,11 @@
       <c r="G34" t="s">
         <v>42</v>
       </c>
-      <c r="I34" s="4" t="s">
-        <v>116</v>
-      </c>
+      <c r="H34" s="8"/>
+      <c r="I34" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J34" s="8"/>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
@@ -1798,13 +2005,13 @@
       <c r="B35" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
       <c r="D35" t="s">
         <v>6</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E35" s="5" t="s">
         <v>72</v>
       </c>
       <c r="F35" t="s">
@@ -1813,6 +2020,13 @@
       <c r="G35" t="s">
         <v>72</v>
       </c>
+      <c r="H35" s="13">
+        <v>42402</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="J35" s="8"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
@@ -1821,13 +2035,13 @@
       <c r="B36" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="7" t="s">
         <v>73</v>
       </c>
       <c r="D36" t="s">
         <v>6</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F36" t="s">
@@ -1836,6 +2050,13 @@
       <c r="G36" t="s">
         <v>23</v>
       </c>
+      <c r="H36" s="13">
+        <v>41116</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="J36" s="8"/>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
@@ -1844,13 +2065,13 @@
       <c r="B37" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="7" t="s">
         <v>74</v>
       </c>
       <c r="D37" t="s">
         <v>6</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E37" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F37" t="s">
@@ -1859,9 +2080,11 @@
       <c r="G37" t="s">
         <v>42</v>
       </c>
-      <c r="I37" s="4" t="s">
-        <v>116</v>
-      </c>
+      <c r="H37" s="8"/>
+      <c r="I37" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J37" s="8"/>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
@@ -1870,13 +2093,13 @@
       <c r="B38" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="7" t="s">
         <v>75</v>
       </c>
       <c r="D38" t="s">
         <v>6</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="E38" s="5" t="s">
         <v>39</v>
       </c>
       <c r="F38" t="s">
@@ -1885,15 +2108,13 @@
       <c r="G38" t="s">
         <v>31</v>
       </c>
-      <c r="H38" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>145</v>
-      </c>
+      <c r="H38" s="14">
+        <v>39681</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J38" s="3"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
@@ -1902,13 +2123,13 @@
       <c r="B39" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="7" t="s">
         <v>77</v>
       </c>
       <c r="D39" t="s">
         <v>6</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="E39" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F39" t="s">
@@ -1917,12 +2138,13 @@
       <c r="G39" t="s">
         <v>78</v>
       </c>
-      <c r="H39" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>159</v>
-      </c>
+      <c r="H39" s="11">
+        <v>39904</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="J39" s="8"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
@@ -1931,13 +2153,13 @@
       <c r="B40" t="s">
         <v>83</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="7" t="s">
         <v>83</v>
       </c>
       <c r="D40" t="s">
         <v>6</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="E40" s="5" t="s">
         <v>84</v>
       </c>
       <c r="F40" t="s">
@@ -1946,6 +2168,11 @@
       <c r="G40" t="s">
         <v>23</v>
       </c>
+      <c r="H40" s="8"/>
+      <c r="I40" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="J40" s="8"/>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
@@ -1954,13 +2181,13 @@
       <c r="B41" t="s">
         <v>79</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="7" t="s">
         <v>79</v>
       </c>
       <c r="D41" t="s">
         <v>5</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="E41" s="5" t="s">
         <v>80</v>
       </c>
       <c r="F41" t="s">
@@ -1969,9 +2196,11 @@
       <c r="G41" t="s">
         <v>82</v>
       </c>
-      <c r="I41" s="4" t="s">
-        <v>116</v>
-      </c>
+      <c r="H41" s="8"/>
+      <c r="I41" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J41" s="8"/>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
@@ -1980,13 +2209,13 @@
       <c r="B42" t="s">
         <v>85</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="7" t="s">
         <v>85</v>
       </c>
       <c r="D42" t="s">
         <v>6</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="E42" s="5" t="s">
         <v>78</v>
       </c>
       <c r="F42" t="s">
@@ -1995,14 +2224,14 @@
       <c r="G42" t="s">
         <v>78</v>
       </c>
-      <c r="H42" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="J42" s="4" t="s">
-        <v>161</v>
+      <c r="H42" s="13">
+        <v>41944</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2012,13 +2241,13 @@
       <c r="B43" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="7" t="s">
         <v>86</v>
       </c>
       <c r="D43" t="s">
         <v>6</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E43" s="5" t="s">
         <v>87</v>
       </c>
       <c r="F43" t="s">
@@ -2027,12 +2256,13 @@
       <c r="G43" t="s">
         <v>89</v>
       </c>
-      <c r="H43" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>158</v>
-      </c>
+      <c r="H43" s="11">
+        <v>39791</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="J43" s="8"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
@@ -2041,13 +2271,13 @@
       <c r="B44" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="7" t="s">
         <v>90</v>
       </c>
       <c r="D44" t="s">
         <v>6</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="E44" s="5" t="s">
         <v>91</v>
       </c>
       <c r="F44" t="s">
@@ -2056,6 +2286,9 @@
       <c r="G44" t="s">
         <v>91</v>
       </c>
+      <c r="H44" s="15"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
@@ -2064,13 +2297,13 @@
       <c r="B45" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="7" t="s">
         <v>92</v>
       </c>
       <c r="D45" t="s">
         <v>6</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="E45" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F45" t="s">
@@ -2079,6 +2312,13 @@
       <c r="G45" t="s">
         <v>42</v>
       </c>
+      <c r="H45" s="13">
+        <v>39234</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J45" s="8"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
@@ -2087,13 +2327,13 @@
       <c r="B46" t="s">
         <v>93</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="7" t="s">
         <v>93</v>
       </c>
       <c r="D46" t="s">
         <v>6</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="E46" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F46" t="s">
@@ -2102,9 +2342,11 @@
       <c r="G46" t="s">
         <v>42</v>
       </c>
-      <c r="I46" s="4" t="s">
-        <v>116</v>
-      </c>
+      <c r="H46" s="8"/>
+      <c r="I46" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J46" s="8"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
@@ -2113,13 +2355,13 @@
       <c r="B47" t="s">
         <v>94</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="7" t="s">
         <v>94</v>
       </c>
       <c r="D47" t="s">
         <v>6</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="E47" s="5" t="s">
         <v>95</v>
       </c>
       <c r="F47" t="s">
@@ -2128,7 +2370,9 @@
       <c r="G47" t="s">
         <v>95</v>
       </c>
-      <c r="H47" s="10"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
@@ -2137,13 +2381,13 @@
       <c r="B48" t="s">
         <v>96</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="7" t="s">
         <v>96</v>
       </c>
       <c r="D48" t="s">
         <v>6</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="E48" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F48" t="s">
@@ -2152,22 +2396,28 @@
       <c r="G48" t="s">
         <v>23</v>
       </c>
-      <c r="I48" s="2"/>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="H48" s="13">
+        <v>41071</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="J48" s="8"/>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
         <v>15</v>
       </c>
       <c r="B49" t="s">
         <v>97</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D49" t="s">
         <v>6</v>
       </c>
-      <c r="E49" s="6" t="s">
+      <c r="E49" s="5" t="s">
         <v>54</v>
       </c>
       <c r="F49" t="s">
@@ -2176,21 +2426,24 @@
       <c r="G49" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" t="s">
         <v>7</v>
       </c>
       <c r="B50" t="s">
         <v>98</v>
       </c>
-      <c r="C50" s="11" t="s">
-        <v>135</v>
+      <c r="C50" s="7" t="s">
+        <v>130</v>
       </c>
       <c r="D50" t="s">
         <v>6</v>
       </c>
-      <c r="E50" s="6" t="s">
+      <c r="E50" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F50" t="s">
@@ -2199,21 +2452,28 @@
       <c r="G50" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="H50" s="13">
+        <v>40544</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="J50" s="8"/>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" t="s">
         <v>15</v>
       </c>
       <c r="B51" t="s">
         <v>99</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="7" t="s">
         <v>99</v>
       </c>
       <c r="D51" t="s">
         <v>6</v>
       </c>
-      <c r="E51" s="6" t="s">
+      <c r="E51" s="5" t="s">
         <v>100</v>
       </c>
       <c r="F51" t="s">
@@ -2222,22 +2482,28 @@
       <c r="G51" t="s">
         <v>78</v>
       </c>
-      <c r="I51" s="2"/>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="H51" s="13">
+        <v>41395</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="J51" s="8"/>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" t="s">
         <v>15</v>
       </c>
       <c r="B52" t="s">
         <v>101</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="7" t="s">
         <v>101</v>
       </c>
       <c r="D52" t="s">
         <v>6</v>
       </c>
-      <c r="E52" s="6" t="s">
+      <c r="E52" s="5" t="s">
         <v>54</v>
       </c>
       <c r="F52" t="s">
@@ -2246,21 +2512,24 @@
       <c r="G52" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" t="s">
         <v>7</v>
       </c>
       <c r="B53" t="s">
         <v>102</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C53" s="7" t="s">
         <v>102</v>
       </c>
       <c r="D53" t="s">
         <v>6</v>
       </c>
-      <c r="E53" s="6" t="s">
+      <c r="E53" s="5" t="s">
         <v>78</v>
       </c>
       <c r="F53" t="s">
@@ -2269,21 +2538,28 @@
       <c r="G53" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="H53" s="13">
+        <v>41913</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="J53" s="8"/>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54" t="s">
         <v>15</v>
       </c>
       <c r="B54" t="s">
         <v>103</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="7" t="s">
         <v>103</v>
       </c>
       <c r="D54" t="s">
         <v>6</v>
       </c>
-      <c r="E54" s="6" t="s">
+      <c r="E54" s="5" t="s">
         <v>54</v>
       </c>
       <c r="F54" t="s">
@@ -2292,24 +2568,26 @@
       <c r="G54" t="s">
         <v>40</v>
       </c>
-      <c r="I54" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
+      <c r="H54" s="8"/>
+      <c r="I54" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J54" s="8"/>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" t="s">
         <v>15</v>
       </c>
       <c r="B55" t="s">
         <v>105</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="C55" s="7" t="s">
         <v>105</v>
       </c>
       <c r="D55" t="s">
         <v>6</v>
       </c>
-      <c r="E55" s="6" t="s">
+      <c r="E55" s="5" t="s">
         <v>54</v>
       </c>
       <c r="F55" t="s">
@@ -2318,21 +2596,24 @@
       <c r="G55" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="8"/>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56" t="s">
         <v>15</v>
       </c>
       <c r="B56" t="s">
         <v>106</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="C56" s="7" t="s">
         <v>106</v>
       </c>
       <c r="D56" t="s">
         <v>6</v>
       </c>
-      <c r="E56" s="6" t="s">
+      <c r="E56" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F56" t="s">
@@ -2341,21 +2622,24 @@
       <c r="G56" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="57" spans="1:9">
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8"/>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" t="s">
         <v>15</v>
       </c>
       <c r="B57" t="s">
         <v>107</v>
       </c>
-      <c r="C57" s="11" t="s">
-        <v>140</v>
+      <c r="C57" s="7" t="s">
+        <v>135</v>
       </c>
       <c r="D57" t="s">
         <v>6</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="E57" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F57" t="s">
@@ -2364,21 +2648,28 @@
       <c r="G57" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="H57" s="13">
+        <v>40848</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="J57" s="8"/>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" t="s">
         <v>15</v>
       </c>
       <c r="B58" t="s">
         <v>108</v>
       </c>
-      <c r="C58" s="11" t="s">
-        <v>138</v>
+      <c r="C58" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="D58" t="s">
         <v>6</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="E58" s="5" t="s">
         <v>109</v>
       </c>
       <c r="F58" t="s">
@@ -2387,21 +2678,28 @@
       <c r="G58" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="H58" s="13">
+        <v>40837</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="J58" s="8"/>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" t="s">
         <v>27</v>
       </c>
       <c r="B59" t="s">
         <v>110</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" s="7" t="s">
         <v>110</v>
       </c>
       <c r="D59" t="s">
         <v>6</v>
       </c>
-      <c r="E59" s="6" t="s">
+      <c r="E59" s="5" t="s">
         <v>69</v>
       </c>
       <c r="F59" t="s">
@@ -2410,23 +2708,28 @@
       <c r="G59" t="s">
         <v>69</v>
       </c>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="H59" s="13">
+        <v>41214</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="J59" s="8"/>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" t="s">
         <v>7</v>
       </c>
       <c r="B60" t="s">
         <v>111</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="C60" s="7" t="s">
         <v>111</v>
       </c>
       <c r="D60" t="s">
         <v>6</v>
       </c>
-      <c r="E60" s="6" t="s">
+      <c r="E60" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F60" t="s">
@@ -2435,6 +2738,9 @@
       <c r="G60" t="s">
         <v>23</v>
       </c>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:I60" xr:uid="{C4318D23-DF38-43A2-8A39-EA73F623CF41}">
@@ -2446,32 +2752,55 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="I54" r:id="rId1" xr:uid="{AA189FB5-EB97-4BBD-AE1A-7EC36156D191}"/>
-    <hyperlink ref="I34" r:id="rId2" xr:uid="{318653DA-3323-404B-9BE5-B8F9E1658C26}"/>
-    <hyperlink ref="I25" r:id="rId3" xr:uid="{1101286A-1A3C-4A6B-BB58-E0C63F469CA0}"/>
-    <hyperlink ref="I46" r:id="rId4" xr:uid="{C09CCD63-60AF-4B13-A771-DB0C6E4B61AF}"/>
-    <hyperlink ref="I24" r:id="rId5" xr:uid="{6CE4CE1B-4841-429D-B6A7-6A407F06F6D1}"/>
-    <hyperlink ref="I37" r:id="rId6" xr:uid="{C6E7620E-A1EF-4EFF-84D7-842E7FDBBB4E}"/>
-    <hyperlink ref="I4" r:id="rId7" xr:uid="{5A580499-E36F-4B16-B454-E735AEDB24D7}"/>
-    <hyperlink ref="I41" r:id="rId8" xr:uid="{44E41522-E812-4F3A-9A86-2E3A60D98867}"/>
-    <hyperlink ref="I1" r:id="rId9" display="https://web.archive.org/web/20070607195753/http:/www.env-it.de/luftdaten/download/public/html/Umweltzonen/index.htm" xr:uid="{428FC607-9BFA-4091-AF96-4FBAD7AB8680}"/>
-    <hyperlink ref="I15" r:id="rId10" display="https://web.archive.org/web/20070325091507/http:/www.rp.baden-wuerttemberg.de/servlet/PB/show/1159769/rpf-ref54.1-lrp.pdf" xr:uid="{F444C233-092B-481B-9A46-CC5D89B9EC48}"/>
-    <hyperlink ref="I6" r:id="rId11" xr:uid="{53938316-734B-4493-BD98-0092020B24C8}"/>
-    <hyperlink ref="J6" r:id="rId12" xr:uid="{D89F18F0-01D7-4D4C-9ECC-A580F64F7ACE}"/>
-    <hyperlink ref="I3" r:id="rId13" xr:uid="{D1CE2CAB-DC57-4C6A-B940-5C6E15DA2A08}"/>
-    <hyperlink ref="J3" r:id="rId14" xr:uid="{C6A2F742-9644-4320-9A7D-376290596A05}"/>
-    <hyperlink ref="J38" r:id="rId15" location="2-fortschreibung-des-luftreinhalteplans_13" display="https://www.muenchen.de/rathaus/Stadtverwaltung/Referat-fuer-Gesundheit-und-Umwelt/Luft_und_Strahlung/Luftreinhalteplan.html - 2-fortschreibung-des-luftreinhalteplans_13" xr:uid="{B5A335CA-064B-4D43-8BAD-F073D860D9DC}"/>
-    <hyperlink ref="I28" r:id="rId16" xr:uid="{BA4AF934-06EE-4995-A7C6-2580C1503A33}"/>
-    <hyperlink ref="J28" r:id="rId17" xr:uid="{2749FEE2-BF00-4274-B7DF-5EA7EB307E53}"/>
-    <hyperlink ref="I8" r:id="rId18" xr:uid="{7D56F90E-1E4B-4482-81F9-FCD49BE68261}"/>
-    <hyperlink ref="I18" r:id="rId19" xr:uid="{3C013743-470B-4F05-B9C1-3582B2F51821}"/>
-    <hyperlink ref="I12" r:id="rId20" xr:uid="{4014BD27-873D-44F8-B7FB-9D13C1798518}"/>
-    <hyperlink ref="I43" r:id="rId21" xr:uid="{614EB40E-8487-40DF-AEC5-FD79790069F6}"/>
-    <hyperlink ref="I39" r:id="rId22" xr:uid="{99F92922-FCBB-4BE6-820A-765A34625186}"/>
-    <hyperlink ref="J42" r:id="rId23" xr:uid="{1DDA0C60-77E5-4EBD-AD0B-DCBA4D6A2DF5}"/>
+    <hyperlink ref="I1" r:id="rId1" display="https://web.archive.org/web/20070607195753/http:/www.env-it.de/luftdaten/download/public/html/Umweltzonen/index.htm" xr:uid="{428FC607-9BFA-4091-AF96-4FBAD7AB8680}"/>
+    <hyperlink ref="I54" r:id="rId2" display="https://www.schwarzwald-netz.com/168/Schwarzwald-Anreise/Umwelt-Zonen-und-Schadstoffplaketten-Schwarzwald.html" xr:uid="{5269E172-270B-4B16-9EF4-81AE3BA25A1B}"/>
+    <hyperlink ref="I34" r:id="rId3" display="https://www.schwarzwald-netz.com/168/Schwarzwald-Anreise/Umwelt-Zonen-und-Schadstoffplaketten-Schwarzwald.html" xr:uid="{28F934D0-E450-4A38-ACD0-81C267124DC7}"/>
+    <hyperlink ref="I25" r:id="rId4" display="https://www.schwarzwald-netz.com/168/Schwarzwald-Anreise/Umwelt-Zonen-und-Schadstoffplaketten-Schwarzwald.html" xr:uid="{D3CB5928-68C9-4ACD-8D5F-14DC5E413153}"/>
+    <hyperlink ref="I46" r:id="rId5" display="https://www.schwarzwald-netz.com/168/Schwarzwald-Anreise/Umwelt-Zonen-und-Schadstoffplaketten-Schwarzwald.html" xr:uid="{118FF6C7-DBAE-485E-B77A-A45AE5532386}"/>
+    <hyperlink ref="I24" r:id="rId6" display="https://www.schwarzwald-netz.com/168/Schwarzwald-Anreise/Umwelt-Zonen-und-Schadstoffplaketten-Schwarzwald.html" xr:uid="{1764224C-2808-44ED-891B-D9CC700E9C72}"/>
+    <hyperlink ref="I37" r:id="rId7" display="https://www.schwarzwald-netz.com/168/Schwarzwald-Anreise/Umwelt-Zonen-und-Schadstoffplaketten-Schwarzwald.html" xr:uid="{A7B04BB9-7105-438F-969B-C6EDB707D621}"/>
+    <hyperlink ref="I4" r:id="rId8" display="https://www.schwarzwald-netz.com/168/Schwarzwald-Anreise/Umwelt-Zonen-und-Schadstoffplaketten-Schwarzwald.html" xr:uid="{27558769-51CD-43C2-ABE6-3163BD4B15FB}"/>
+    <hyperlink ref="I41" r:id="rId9" display="https://www.schwarzwald-netz.com/168/Schwarzwald-Anreise/Umwelt-Zonen-und-Schadstoffplaketten-Schwarzwald.html" xr:uid="{50B7AEDC-844B-4AEB-B5CF-05BC646CFDA3}"/>
+    <hyperlink ref="I15" r:id="rId10" display="https://web.archive.org/web/20070325091507/http:/www.rp.baden-wuerttemberg.de/servlet/PB/show/1159769/rpf-ref54.1-lrp.pdf" xr:uid="{3C8501D2-DC8F-4BFB-A9AA-8681458FD737}"/>
+    <hyperlink ref="I6" r:id="rId11" display="https://www.berlin.de/senuvk/umwelt/luftqualitaet/de/luftreinhalteplan/download/2005/anpassung_aktionsplan_umweltzone.pdf" xr:uid="{7FCAEBC1-1CBE-423E-A056-42132F74C350}"/>
+    <hyperlink ref="J6" r:id="rId12" display="https://www.berlin.de/senuvk/umwelt/luftqualitaet/de/luftreinhalteplan/doku_lrp_2005_2010.shtml" xr:uid="{5091515C-3E9D-40E0-BE67-037397F7DD43}"/>
+    <hyperlink ref="I3" r:id="rId13" display="http://www.aachen.de/DE/stadt_buerger/umwelt/luft-stadtklima/luftreinhalteplan_umweltzone/umweltzone/pressemitteilungen/presseinfo_2015_01_20.html" xr:uid="{1ABB6FE7-4350-47B4-AEDA-813DC65E0A87}"/>
+    <hyperlink ref="J3" r:id="rId14" display="http://www.aachen.de/DE/stadt_buerger/umwelt/luft-stadtklima/luftreinhalteplan_umweltzone/umweltzone/pressemitteilungen/index.html" xr:uid="{2C429C93-A534-48C3-9600-E484AEAE9854}"/>
+    <hyperlink ref="I28" r:id="rId15" display="https://static.leipzig.de/fileadmin/mediendatenbank/leipzig-de/Stadt/02.3_Dez3_Umwelt_Ordnung_Sport/36_Amt_fuer_Umweltschutz/Luft_und_Laerm/Luftreinhaltung/Luftreinhalteplan/Luftreinhalteplan_2009.pdf" xr:uid="{2B0D22BA-6E78-4BAE-85EE-FB7CB6EE6281}"/>
+    <hyperlink ref="I8" r:id="rId16" display="https://www.bauumwelt.bremen.de/umwelt/luft/umweltzone_bremen-24570" xr:uid="{6E683047-08A2-4C7E-81D8-C56A063B62AF}"/>
+    <hyperlink ref="I18" r:id="rId17" display="https://www.umwelt.niedersachsen.de/startseite/themen/luftqualitat/luftschadstoffberechnungen_amp_luftreinhalteplane/luftreinhalteplane/lrp_hannover/luftreinhalteplan-fuer-hannover-8921.html" xr:uid="{5AD0A83F-EFC9-4727-90ED-8A6CCED2D44A}"/>
+    <hyperlink ref="I12" r:id="rId18" display="https://www.erfurt.de/ef/de/leben/verkehr/mobil/auto/umweltzone/index.html" xr:uid="{DFF82A51-8AE5-4946-8081-9633D49FA593}"/>
+    <hyperlink ref="I43" r:id="rId19" display="https://www.osnabrueck.de/umweltzone/" xr:uid="{254C8565-6A79-4BC9-B5EA-B5D105A84252}"/>
+    <hyperlink ref="J42" r:id="rId20" display="https://www.offenbach.de/leben-in-of/umwelt-klimaschutz/Luft_Laerm/Luftreinhaltung/testartikel-umweltzone.php" xr:uid="{499AE478-AE18-4703-B9A2-C9F8836F1CA9}"/>
+    <hyperlink ref="J7" r:id="rId21" xr:uid="{0421FD74-C803-473C-88F5-086AE690A0AC}"/>
+    <hyperlink ref="I35" r:id="rId22" xr:uid="{628F2A74-145C-49DE-B4FB-AC3932E97718}"/>
+    <hyperlink ref="I9" r:id="rId23" xr:uid="{C39E01F0-DBA5-40AC-8802-4C4E35AF0427}"/>
+    <hyperlink ref="I53" r:id="rId24" xr:uid="{73063BA1-F10F-4E2C-BE7B-4131453C32F7}"/>
+    <hyperlink ref="I29" r:id="rId25" xr:uid="{C98B85BB-926F-4DAD-BCB3-F8E9B0140427}"/>
+    <hyperlink ref="I51" r:id="rId26" xr:uid="{E362FDA4-E1A7-4A5F-8373-0E69550B1868}"/>
+    <hyperlink ref="I58" r:id="rId27" xr:uid="{F3003EE1-0C9E-4A61-999F-3B609C3FAAC8}"/>
+    <hyperlink ref="I33" r:id="rId28" xr:uid="{72096BF0-CB94-4553-A05E-B623A81DF74F}"/>
+    <hyperlink ref="I59" r:id="rId29" xr:uid="{30318F0A-CE4F-4117-AAB6-6C28A6B22D92}"/>
+    <hyperlink ref="I27" r:id="rId30" xr:uid="{D5B7B554-5084-40B4-A794-96B553B7BD82}"/>
+    <hyperlink ref="I31" r:id="rId31" xr:uid="{A4D4E947-51D8-41CB-87CC-5610BF87A105}"/>
+    <hyperlink ref="I36" r:id="rId32" xr:uid="{56848BE7-5899-4333-8105-0FD39B1F1B5C}"/>
+    <hyperlink ref="I48" r:id="rId33" xr:uid="{D86F42E5-A4DB-444A-9A6D-0F95DDD87AE4}"/>
+    <hyperlink ref="I16" r:id="rId34" xr:uid="{384A9BE1-978F-4EA5-91DE-63D8BD23D96C}"/>
+    <hyperlink ref="I20" r:id="rId35" xr:uid="{ACF4D823-C481-4AEC-8532-F41BF69ABA7A}"/>
+    <hyperlink ref="J25" r:id="rId36" xr:uid="{9964B3ED-3FF5-485E-92F5-34CC48D46C2A}"/>
+    <hyperlink ref="I57" r:id="rId37" xr:uid="{22672795-E2B5-4695-9B8D-F7EFBAE3DEBD}"/>
+    <hyperlink ref="J27" r:id="rId38" xr:uid="{3843EDBB-C9D2-4F28-8990-61E8179A8382}"/>
+    <hyperlink ref="J28" r:id="rId39" xr:uid="{5AB71D97-850E-459C-8CC2-00D5BD60776B}"/>
+    <hyperlink ref="J29" r:id="rId40" xr:uid="{89E75AF6-7EEC-4B1E-AAC4-620A37E9FE8E}"/>
+    <hyperlink ref="I39" r:id="rId41" xr:uid="{B0969789-C1CD-40F4-9887-036E27B22992}"/>
+    <hyperlink ref="I26" r:id="rId42" xr:uid="{3B62E6D7-8C4E-4D66-89A2-A4C087C24528}"/>
+    <hyperlink ref="J32" r:id="rId43" xr:uid="{0250B234-66F2-4511-992F-C3B52A246482}"/>
+    <hyperlink ref="I7" r:id="rId44" xr:uid="{45B478C6-0394-4A28-A049-C90955215965}"/>
+    <hyperlink ref="I19" r:id="rId45" xr:uid="{C9EA2844-B713-481C-B0F7-B00B07004AB7}"/>
+    <hyperlink ref="I45" r:id="rId46" xr:uid="{E416A674-A008-43BE-9126-A099AC307EDE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId24"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId47"/>
 </worksheet>
 </file>
 
@@ -2489,73 +2818,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="2" spans="2:3">
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>39237</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>118</v>
+      <c r="C2" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="2:3">
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>39240</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>117</v>
+      <c r="C3" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="2:3">
       <c r="B9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="2:3">
       <c r="B10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="2:3">
       <c r="B11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="2:3">
       <c r="B13" t="s">
-        <v>131</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>132</v>
+        <v>126</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2568,4 +2897,1735 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBFBC39D-83BB-483C-BFB7-D0283EED5A33}">
+  <dimension ref="A1:J60"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:J60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="25.6328125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="11.6328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="I1" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="5">
+        <v>42401</v>
+      </c>
+      <c r="F3" s="5">
+        <v>42401</v>
+      </c>
+      <c r="G3" s="5">
+        <v>42401</v>
+      </c>
+      <c r="H3" s="11">
+        <v>42297</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="5">
+        <v>39995</v>
+      </c>
+      <c r="F4" s="5">
+        <v>40544</v>
+      </c>
+      <c r="G4" s="5">
+        <v>42522</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="16">
+        <v>42826</v>
+      </c>
+      <c r="F5" s="16">
+        <v>42826</v>
+      </c>
+      <c r="G5" s="16">
+        <v>42826</v>
+      </c>
+      <c r="H5" s="15"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="6">
+        <v>39448</v>
+      </c>
+      <c r="F6" s="5">
+        <v>40179</v>
+      </c>
+      <c r="G6" s="5">
+        <v>40179</v>
+      </c>
+      <c r="H6" s="11">
+        <v>39161</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="5">
+        <v>40179</v>
+      </c>
+      <c r="F7" s="5">
+        <v>41091</v>
+      </c>
+      <c r="G7" s="5">
+        <v>41821</v>
+      </c>
+      <c r="H7" s="5">
+        <v>40087</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="6">
+        <v>39814</v>
+      </c>
+      <c r="F8" s="5">
+        <v>40179</v>
+      </c>
+      <c r="G8" s="5">
+        <v>40725</v>
+      </c>
+      <c r="H8" s="12">
+        <v>38930</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="5">
+        <v>42309</v>
+      </c>
+      <c r="F9" s="5">
+        <v>42309</v>
+      </c>
+      <c r="G9" s="5">
+        <v>42309</v>
+      </c>
+      <c r="H9" s="14">
+        <v>42010</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="5">
+        <v>40725</v>
+      </c>
+      <c r="F10" s="5">
+        <v>40725</v>
+      </c>
+      <c r="G10" s="5">
+        <v>41183</v>
+      </c>
+      <c r="H10" s="13">
+        <v>40459</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="5">
+        <v>39859</v>
+      </c>
+      <c r="F11" s="5">
+        <v>40603</v>
+      </c>
+      <c r="G11" s="5">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="5">
+        <v>41183</v>
+      </c>
+      <c r="F12" s="5">
+        <v>41183</v>
+      </c>
+      <c r="G12" s="5">
+        <v>41183</v>
+      </c>
+      <c r="H12" s="11">
+        <v>41192</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="5">
+        <v>42522</v>
+      </c>
+      <c r="F13" s="5">
+        <v>42522</v>
+      </c>
+      <c r="G13" s="5">
+        <v>42522</v>
+      </c>
+      <c r="H13" s="13">
+        <v>42461</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="5">
+        <v>39722</v>
+      </c>
+      <c r="F14" s="5">
+        <v>40179</v>
+      </c>
+      <c r="G14" s="5">
+        <v>40909</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="5">
+        <v>40179</v>
+      </c>
+      <c r="F15" s="5">
+        <v>40909</v>
+      </c>
+      <c r="G15" s="5">
+        <v>41275</v>
+      </c>
+      <c r="H15" s="12">
+        <v>38777</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="5">
+        <v>40909</v>
+      </c>
+      <c r="F16" s="5">
+        <v>41275</v>
+      </c>
+      <c r="G16" s="5">
+        <v>41821</v>
+      </c>
+      <c r="H16" s="14">
+        <v>40856</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="5">
+        <v>40787</v>
+      </c>
+      <c r="F17" s="5">
+        <v>40787</v>
+      </c>
+      <c r="G17" s="5">
+        <v>41275</v>
+      </c>
+      <c r="H17" s="13">
+        <v>40664</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="5">
+        <v>39448</v>
+      </c>
+      <c r="F18" s="5">
+        <v>39814</v>
+      </c>
+      <c r="G18" s="5">
+        <v>40179</v>
+      </c>
+      <c r="H18" s="12">
+        <v>39264</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="5">
+        <v>40179</v>
+      </c>
+      <c r="F19" s="5">
+        <v>40909</v>
+      </c>
+      <c r="G19" s="5">
+        <v>41275</v>
+      </c>
+      <c r="H19" s="13">
+        <v>38758</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="5">
+        <v>40909</v>
+      </c>
+      <c r="F20" s="5">
+        <v>40909</v>
+      </c>
+      <c r="G20" s="5">
+        <v>41275</v>
+      </c>
+      <c r="H20" s="13">
+        <v>40848</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="5">
+        <v>39814</v>
+      </c>
+      <c r="F21" s="5">
+        <v>40909</v>
+      </c>
+      <c r="G21" s="5">
+        <v>41275</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="5">
+        <v>39814</v>
+      </c>
+      <c r="F22" s="5">
+        <v>40909</v>
+      </c>
+      <c r="G22" s="5">
+        <v>41275</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="5">
+        <v>39508</v>
+      </c>
+      <c r="F23" s="5">
+        <v>40909</v>
+      </c>
+      <c r="G23" s="5">
+        <v>41275</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="5">
+        <v>39814</v>
+      </c>
+      <c r="F24" s="5">
+        <v>40909</v>
+      </c>
+      <c r="G24" s="5">
+        <v>41275</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="5">
+        <v>39448</v>
+      </c>
+      <c r="F25" s="5">
+        <v>41275</v>
+      </c>
+      <c r="G25" s="5">
+        <v>41821</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="5">
+        <v>40544</v>
+      </c>
+      <c r="F26" s="5">
+        <v>40544</v>
+      </c>
+      <c r="G26" s="5">
+        <v>41091</v>
+      </c>
+      <c r="H26" s="5">
+        <v>40452</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="5">
+        <v>41275</v>
+      </c>
+      <c r="F27" s="5">
+        <v>41275</v>
+      </c>
+      <c r="G27" s="5">
+        <v>41821</v>
+      </c>
+      <c r="H27" s="13">
+        <v>41153</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="5">
+        <v>40603</v>
+      </c>
+      <c r="F28" s="5">
+        <v>40603</v>
+      </c>
+      <c r="G28" s="5">
+        <v>40603</v>
+      </c>
+      <c r="H28" s="12">
+        <v>40165</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="5">
+        <v>41610</v>
+      </c>
+      <c r="F29" s="5">
+        <v>41610</v>
+      </c>
+      <c r="G29" s="5">
+        <v>41610</v>
+      </c>
+      <c r="H29" s="13">
+        <v>40695</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="16">
+        <v>43131</v>
+      </c>
+      <c r="F30" s="16">
+        <v>43131</v>
+      </c>
+      <c r="G30" s="16">
+        <v>43131</v>
+      </c>
+      <c r="H30" s="15"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="5">
+        <v>41275</v>
+      </c>
+      <c r="F31" s="5">
+        <v>41275</v>
+      </c>
+      <c r="G31" s="5">
+        <v>41275</v>
+      </c>
+      <c r="H31" s="13">
+        <v>41183</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="5">
+        <v>40787</v>
+      </c>
+      <c r="F32" s="5">
+        <v>40787</v>
+      </c>
+      <c r="G32" s="5">
+        <v>41275</v>
+      </c>
+      <c r="H32" s="13">
+        <v>40645</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="5">
+        <v>41306</v>
+      </c>
+      <c r="F33" s="5">
+        <v>41306</v>
+      </c>
+      <c r="G33" s="5">
+        <v>41306</v>
+      </c>
+      <c r="H33" s="13">
+        <v>40264</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="5">
+        <v>39508</v>
+      </c>
+      <c r="F34" s="5">
+        <v>40909</v>
+      </c>
+      <c r="G34" s="5">
+        <v>41275</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="5">
+        <v>42461</v>
+      </c>
+      <c r="F35" s="5">
+        <v>42461</v>
+      </c>
+      <c r="G35" s="5">
+        <v>42461</v>
+      </c>
+      <c r="H35" s="13">
+        <v>42402</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="5">
+        <v>41275</v>
+      </c>
+      <c r="F36" s="5">
+        <v>41275</v>
+      </c>
+      <c r="G36" s="5">
+        <v>41821</v>
+      </c>
+      <c r="H36" s="13">
+        <v>41116</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="5">
+        <v>39814</v>
+      </c>
+      <c r="F37" s="5">
+        <v>40909</v>
+      </c>
+      <c r="G37" s="5">
+        <v>41275</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="5">
+        <v>39722</v>
+      </c>
+      <c r="F38" s="5">
+        <v>40452</v>
+      </c>
+      <c r="G38" s="5">
+        <v>41183</v>
+      </c>
+      <c r="H38" s="14">
+        <v>39681</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="5">
+        <v>40179</v>
+      </c>
+      <c r="F39" s="5">
+        <v>40179</v>
+      </c>
+      <c r="G39" s="5">
+        <v>42005</v>
+      </c>
+      <c r="H39" s="11">
+        <v>39904</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="5">
+        <v>40224</v>
+      </c>
+      <c r="F40" s="5">
+        <v>40603</v>
+      </c>
+      <c r="G40" s="5">
+        <v>41821</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="5">
+        <v>40118</v>
+      </c>
+      <c r="F41" s="5">
+        <v>41218</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="5">
+        <v>42005</v>
+      </c>
+      <c r="F42" s="5">
+        <v>42005</v>
+      </c>
+      <c r="G42" s="5">
+        <v>42005</v>
+      </c>
+      <c r="H42" s="13">
+        <v>41944</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="5">
+        <v>40182</v>
+      </c>
+      <c r="F43" s="5">
+        <v>40546</v>
+      </c>
+      <c r="G43" s="5">
+        <v>40911</v>
+      </c>
+      <c r="H43" s="11">
+        <v>39791</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="16">
+        <v>43009</v>
+      </c>
+      <c r="F44" s="16">
+        <v>43009</v>
+      </c>
+      <c r="G44" s="16">
+        <v>43009</v>
+      </c>
+      <c r="H44" s="15"/>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" s="5">
+        <v>40179</v>
+      </c>
+      <c r="F45" s="5">
+        <v>40909</v>
+      </c>
+      <c r="G45" s="5">
+        <v>41275</v>
+      </c>
+      <c r="H45" s="13">
+        <v>39234</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" s="5">
+        <v>39814</v>
+      </c>
+      <c r="F46" s="5">
+        <v>40909</v>
+      </c>
+      <c r="G46" s="5">
+        <v>41275</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="16">
+        <v>43115</v>
+      </c>
+      <c r="F47" s="16">
+        <v>43115</v>
+      </c>
+      <c r="G47" s="16">
+        <v>43115</v>
+      </c>
+      <c r="H47" s="15"/>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="5">
+        <v>41275</v>
+      </c>
+      <c r="F48" s="5">
+        <v>41275</v>
+      </c>
+      <c r="G48" s="5">
+        <v>41821</v>
+      </c>
+      <c r="H48" s="13">
+        <v>41071</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" s="5">
+        <v>39508</v>
+      </c>
+      <c r="F49" s="5">
+        <v>40909</v>
+      </c>
+      <c r="G49" s="5">
+        <v>41275</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" s="5">
+        <v>40909</v>
+      </c>
+      <c r="F50" s="5">
+        <v>41275</v>
+      </c>
+      <c r="G50" s="5">
+        <v>41821</v>
+      </c>
+      <c r="H50" s="13">
+        <v>40544</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="5">
+        <v>41456</v>
+      </c>
+      <c r="F51" s="5">
+        <v>41456</v>
+      </c>
+      <c r="G51" s="5">
+        <v>42005</v>
+      </c>
+      <c r="H51" s="13">
+        <v>41395</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="5">
+        <v>39508</v>
+      </c>
+      <c r="F52" s="5">
+        <v>40909</v>
+      </c>
+      <c r="G52" s="5">
+        <v>41275</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="5">
+        <v>42005</v>
+      </c>
+      <c r="F53" s="5">
+        <v>42005</v>
+      </c>
+      <c r="G53" s="5">
+        <v>42005</v>
+      </c>
+      <c r="H53" s="13">
+        <v>41913</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="5">
+        <v>39508</v>
+      </c>
+      <c r="F54" s="5">
+        <v>40360</v>
+      </c>
+      <c r="G54" s="5">
+        <v>40909</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="5">
+        <v>39508</v>
+      </c>
+      <c r="F55" s="5">
+        <v>40909</v>
+      </c>
+      <c r="G55" s="5">
+        <v>41275</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="5">
+        <v>39814</v>
+      </c>
+      <c r="F56" s="5">
+        <v>40909</v>
+      </c>
+      <c r="G56" s="5">
+        <v>41275</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" s="5">
+        <v>40909</v>
+      </c>
+      <c r="F57" s="5">
+        <v>40909</v>
+      </c>
+      <c r="G57" s="5">
+        <v>41275</v>
+      </c>
+      <c r="H57" s="13">
+        <v>40848</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" s="5">
+        <v>41366</v>
+      </c>
+      <c r="F58" s="5">
+        <v>41366</v>
+      </c>
+      <c r="G58" s="5">
+        <v>41366</v>
+      </c>
+      <c r="H58" s="13">
+        <v>40837</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" s="5">
+        <v>41306</v>
+      </c>
+      <c r="F59" s="5">
+        <v>41306</v>
+      </c>
+      <c r="G59" s="5">
+        <v>41306</v>
+      </c>
+      <c r="H59" s="13">
+        <v>41214</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" s="5">
+        <v>39859</v>
+      </c>
+      <c r="F60" s="5">
+        <v>40603</v>
+      </c>
+      <c r="G60" s="5">
+        <v>41821</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A2:I60" xr:uid="{992D4C13-774D-410B-AB0A-2F47200C11D3}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I60">
+      <sortCondition ref="B2:B60"/>
+    </sortState>
+  </autoFilter>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="I54" r:id="rId1" display="https://www.schwarzwald-netz.com/168/Schwarzwald-Anreise/Umwelt-Zonen-und-Schadstoffplaketten-Schwarzwald.html" xr:uid="{D01FEEB1-32D9-45B8-9087-D616E2EEF3BB}"/>
+    <hyperlink ref="I34" r:id="rId2" display="https://www.schwarzwald-netz.com/168/Schwarzwald-Anreise/Umwelt-Zonen-und-Schadstoffplaketten-Schwarzwald.html" xr:uid="{F7FF43DE-846C-4B06-BAA4-9F9B708EE3CD}"/>
+    <hyperlink ref="I25" r:id="rId3" display="https://www.schwarzwald-netz.com/168/Schwarzwald-Anreise/Umwelt-Zonen-und-Schadstoffplaketten-Schwarzwald.html" xr:uid="{AC1987D0-4618-47F1-8AC1-3BA64C7FF91C}"/>
+    <hyperlink ref="I46" r:id="rId4" display="https://www.schwarzwald-netz.com/168/Schwarzwald-Anreise/Umwelt-Zonen-und-Schadstoffplaketten-Schwarzwald.html" xr:uid="{743CB084-7C5A-4878-B6B7-D724FEA14E1A}"/>
+    <hyperlink ref="I24" r:id="rId5" display="https://www.schwarzwald-netz.com/168/Schwarzwald-Anreise/Umwelt-Zonen-und-Schadstoffplaketten-Schwarzwald.html" xr:uid="{6D72AC99-FB16-4EF6-8E0C-8833C5F9CAD5}"/>
+    <hyperlink ref="I37" r:id="rId6" display="https://www.schwarzwald-netz.com/168/Schwarzwald-Anreise/Umwelt-Zonen-und-Schadstoffplaketten-Schwarzwald.html" xr:uid="{AB2C5A48-7D81-4F5E-A82C-480E948B6489}"/>
+    <hyperlink ref="I4" r:id="rId7" display="https://www.schwarzwald-netz.com/168/Schwarzwald-Anreise/Umwelt-Zonen-und-Schadstoffplaketten-Schwarzwald.html" xr:uid="{CACE102F-522C-4999-B8F7-BE64E24CBFC4}"/>
+    <hyperlink ref="I41" r:id="rId8" display="https://www.schwarzwald-netz.com/168/Schwarzwald-Anreise/Umwelt-Zonen-und-Schadstoffplaketten-Schwarzwald.html" xr:uid="{41714C47-C6F0-463C-95A0-46122D13E159}"/>
+    <hyperlink ref="I1" r:id="rId9" display="https://web.archive.org/web/20070607195753/http:/www.env-it.de/luftdaten/download/public/html/Umweltzonen/index.htm" xr:uid="{4F8B9086-D6F1-4099-8FA8-F375442DE26B}"/>
+    <hyperlink ref="I15" r:id="rId10" display="https://web.archive.org/web/20070325091507/http:/www.rp.baden-wuerttemberg.de/servlet/PB/show/1159769/rpf-ref54.1-lrp.pdf" xr:uid="{A812D46E-0F92-47BE-B0B2-9E6935B75D3C}"/>
+    <hyperlink ref="I6" r:id="rId11" display="https://www.berlin.de/senuvk/umwelt/luftqualitaet/de/luftreinhalteplan/download/2005/anpassung_aktionsplan_umweltzone.pdf" xr:uid="{F526124D-1942-4AC5-8E4F-FBF6B69442AE}"/>
+    <hyperlink ref="J6" r:id="rId12" display="https://www.berlin.de/senuvk/umwelt/luftqualitaet/de/luftreinhalteplan/doku_lrp_2005_2010.shtml" xr:uid="{0D7F501F-606D-4640-B781-D42B2319CAF9}"/>
+    <hyperlink ref="I3" r:id="rId13" display="http://www.aachen.de/DE/stadt_buerger/umwelt/luft-stadtklima/luftreinhalteplan_umweltzone/umweltzone/pressemitteilungen/presseinfo_2015_01_20.html" xr:uid="{5D796A4E-C4BC-44AD-AD9C-1EC960940C6D}"/>
+    <hyperlink ref="J3" r:id="rId14" display="http://www.aachen.de/DE/stadt_buerger/umwelt/luft-stadtklima/luftreinhalteplan_umweltzone/umweltzone/pressemitteilungen/index.html" xr:uid="{D2BFF826-4C9E-47F0-8B30-98FED2EA0022}"/>
+    <hyperlink ref="I28" r:id="rId15" display="https://static.leipzig.de/fileadmin/mediendatenbank/leipzig-de/Stadt/02.3_Dez3_Umwelt_Ordnung_Sport/36_Amt_fuer_Umweltschutz/Luft_und_Laerm/Luftreinhaltung/Luftreinhalteplan/Luftreinhalteplan_2009.pdf" xr:uid="{4095D684-4627-43F6-BA60-3CF6A8CB2413}"/>
+    <hyperlink ref="I8" r:id="rId16" display="https://www.bauumwelt.bremen.de/umwelt/luft/umweltzone_bremen-24570" xr:uid="{03A5F8D7-1B67-452C-870D-1128A1F62FCB}"/>
+    <hyperlink ref="I18" r:id="rId17" display="https://www.umwelt.niedersachsen.de/startseite/themen/luftqualitat/luftschadstoffberechnungen_amp_luftreinhalteplane/luftreinhalteplane/lrp_hannover/luftreinhalteplan-fuer-hannover-8921.html" xr:uid="{B13D065A-6610-4848-95EC-426EC15B6D37}"/>
+    <hyperlink ref="I12" r:id="rId18" display="https://www.erfurt.de/ef/de/leben/verkehr/mobil/auto/umweltzone/index.html" xr:uid="{ED5EA17A-2558-49EF-9DBD-D0B217FA29DF}"/>
+    <hyperlink ref="I43" r:id="rId19" display="https://www.osnabrueck.de/umweltzone/" xr:uid="{5C84D8AC-0470-48D1-9E86-4D34D0AA6D05}"/>
+    <hyperlink ref="J42" r:id="rId20" display="https://www.offenbach.de/leben-in-of/umwelt-klimaschutz/Luft_Laerm/Luftreinhaltung/testartikel-umweltzone.php" xr:uid="{EEF0DD42-079F-4888-9B84-5A99EDE00ED2}"/>
+    <hyperlink ref="J7" r:id="rId21" xr:uid="{1149FFD6-D446-4B07-B98E-58D6B57B600B}"/>
+    <hyperlink ref="I35" r:id="rId22" xr:uid="{F43F9091-CF5E-48BA-967A-27438A3622F8}"/>
+    <hyperlink ref="I9" r:id="rId23" xr:uid="{132523AA-952B-490A-A9D1-CCF45E4A4BE8}"/>
+    <hyperlink ref="I53" r:id="rId24" xr:uid="{FBA3FDF7-CD0B-405E-A6EC-6EC99EEA8E56}"/>
+    <hyperlink ref="I29" r:id="rId25" xr:uid="{772D3BE7-4B21-4EC6-95BD-8BF75EFDFBF2}"/>
+    <hyperlink ref="I51" r:id="rId26" xr:uid="{D2B91AF2-62F7-43E6-94C4-CAD5C78CCA25}"/>
+    <hyperlink ref="I58" r:id="rId27" xr:uid="{303ED838-AD67-4A30-971A-3EAC560569FD}"/>
+    <hyperlink ref="I33" r:id="rId28" xr:uid="{CFA7C573-CE05-4E13-BAB8-949BC3A3E1AE}"/>
+    <hyperlink ref="I59" r:id="rId29" xr:uid="{DF4E45E6-B0CE-429F-9FFC-0D00A749FA8B}"/>
+    <hyperlink ref="I27" r:id="rId30" xr:uid="{92604450-C3E9-4744-BB37-531040A2418A}"/>
+    <hyperlink ref="I31" r:id="rId31" xr:uid="{8FDE02B9-DB0D-4E25-8E38-C83C7D87ACF6}"/>
+    <hyperlink ref="I36" r:id="rId32" xr:uid="{C17B1368-39E7-4238-AEFA-DF43D009758A}"/>
+    <hyperlink ref="I48" r:id="rId33" xr:uid="{EEC793E9-4246-4441-8DC6-D0B7A07A1DF2}"/>
+    <hyperlink ref="I16" r:id="rId34" xr:uid="{4895A98E-237F-47A5-973C-F54C76D9D1B4}"/>
+    <hyperlink ref="I20" r:id="rId35" xr:uid="{89A2AEC1-536E-4FF8-8127-D0A3B8438BA5}"/>
+    <hyperlink ref="J25" r:id="rId36" xr:uid="{AA61D88B-ACAA-4876-8A0E-9786D1EB31F1}"/>
+    <hyperlink ref="I57" r:id="rId37" xr:uid="{164DA308-72F9-4536-ACEA-D2010A027822}"/>
+    <hyperlink ref="J27" r:id="rId38" xr:uid="{23FFEAF4-2286-4F49-933A-DC88DE9A0FC4}"/>
+    <hyperlink ref="J28" r:id="rId39" xr:uid="{C62C867A-355D-40D6-9916-BA51BBB1252F}"/>
+    <hyperlink ref="J29" r:id="rId40" xr:uid="{A08A9408-51DB-49B5-822B-20FE11679E82}"/>
+    <hyperlink ref="I39" r:id="rId41" xr:uid="{5CDECE03-CFA1-4A9F-BD3B-F1A75D81ECC8}"/>
+    <hyperlink ref="I26" r:id="rId42" xr:uid="{B4EC3EA8-E328-458C-B910-1BCA116293FC}"/>
+    <hyperlink ref="J32" r:id="rId43" xr:uid="{4AAD70A8-3617-458A-93B6-BC87C704F0D6}"/>
+    <hyperlink ref="I7" r:id="rId44" xr:uid="{FDDFEDB5-8BBF-4BC5-AFDF-8C4780837DBD}"/>
+    <hyperlink ref="I19" r:id="rId45" xr:uid="{5EF332B2-2058-49F3-A471-C9F2DF1D0D5A}"/>
+    <hyperlink ref="I45" r:id="rId46" xr:uid="{D2147327-0CFA-45FD-A93E-9D8ABE9A712F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final notes on document alsdair
</commit_message>
<xml_diff>
--- a/data/umweltbundesamt/umweltzonen.xlsx
+++ b/data/umweltbundesamt/umweltzonen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aavil\OneDrive\Documentos\A - Estudios\LSE_ASDS\Project\Capstone-Project\data\umweltbundesamt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2845596D-02A7-4D16-B510-5B696812B98C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211CEA1F-9F8E-45F6-B3B2-FB88A0AD3820}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -669,16 +669,16 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -996,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1013,15 +1013,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
       <c r="I1" s="3" t="s">
         <v>116</v>
       </c>
@@ -1078,7 +1078,7 @@
       <c r="G3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="9">
         <v>42297</v>
       </c>
       <c r="I3" s="3" t="s">
@@ -1138,7 +1138,7 @@
       <c r="G5" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="15"/>
+      <c r="H5" s="13"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
     </row>
@@ -1164,7 +1164,7 @@
       <c r="G6" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <v>39161</v>
       </c>
       <c r="I6" s="3" t="s">
@@ -1228,7 +1228,7 @@
       <c r="G8" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="10">
         <v>38930</v>
       </c>
       <c r="I8" s="3" t="s">
@@ -1258,7 +1258,7 @@
       <c r="G9" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="12">
         <v>42010</v>
       </c>
       <c r="I9" s="3" t="s">
@@ -1288,7 +1288,7 @@
       <c r="G10" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="11">
         <v>40459</v>
       </c>
       <c r="I10" s="2" t="s">
@@ -1344,7 +1344,7 @@
       <c r="G12" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="9">
         <v>41192</v>
       </c>
       <c r="I12" s="3" t="s">
@@ -1374,7 +1374,7 @@
       <c r="G13" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="11">
         <v>42461</v>
       </c>
       <c r="I13" s="2" t="s">
@@ -1430,7 +1430,7 @@
       <c r="G15" t="s">
         <v>42</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="10">
         <v>38777</v>
       </c>
       <c r="I15" s="3" t="s">
@@ -1460,7 +1460,7 @@
       <c r="G16" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="12">
         <v>40856</v>
       </c>
       <c r="I16" s="3" t="s">
@@ -1490,7 +1490,7 @@
       <c r="G17" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="13">
+      <c r="H17" s="11">
         <v>40664</v>
       </c>
       <c r="I17" s="2" t="s">
@@ -1520,7 +1520,7 @@
       <c r="G18" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="10">
         <v>39264</v>
       </c>
       <c r="I18" s="3" t="s">
@@ -1550,7 +1550,7 @@
       <c r="G19" t="s">
         <v>42</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="11">
         <v>38758</v>
       </c>
       <c r="I19" s="3" t="s">
@@ -1580,7 +1580,7 @@
       <c r="G20" t="s">
         <v>42</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="11">
         <v>40848</v>
       </c>
       <c r="I20" s="3" t="s">
@@ -1778,7 +1778,7 @@
       <c r="G27" t="s">
         <v>23</v>
       </c>
-      <c r="H27" s="13">
+      <c r="H27" s="11">
         <v>41153</v>
       </c>
       <c r="I27" s="3" t="s">
@@ -1810,7 +1810,7 @@
       <c r="G28" t="s">
         <v>34</v>
       </c>
-      <c r="H28" s="12">
+      <c r="H28" s="10">
         <v>40165</v>
       </c>
       <c r="I28" s="3" t="s">
@@ -1842,7 +1842,7 @@
       <c r="G29" t="s">
         <v>62</v>
       </c>
-      <c r="H29" s="13">
+      <c r="H29" s="11">
         <v>40695</v>
       </c>
       <c r="I29" s="3" t="s">
@@ -1874,7 +1874,7 @@
       <c r="G30" t="s">
         <v>64</v>
       </c>
-      <c r="H30" s="15"/>
+      <c r="H30" s="13"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
     </row>
@@ -1900,7 +1900,7 @@
       <c r="G31" t="s">
         <v>42</v>
       </c>
-      <c r="H31" s="13">
+      <c r="H31" s="11">
         <v>41183</v>
       </c>
       <c r="I31" s="3" t="s">
@@ -1930,7 +1930,7 @@
       <c r="G32" t="s">
         <v>42</v>
       </c>
-      <c r="H32" s="13">
+      <c r="H32" s="11">
         <v>40645</v>
       </c>
       <c r="I32" s="2" t="s">
@@ -1962,7 +1962,7 @@
       <c r="G33" t="s">
         <v>69</v>
       </c>
-      <c r="H33" s="13">
+      <c r="H33" s="11">
         <v>40264</v>
       </c>
       <c r="I33" s="3" t="s">
@@ -2020,7 +2020,7 @@
       <c r="G35" t="s">
         <v>72</v>
       </c>
-      <c r="H35" s="13">
+      <c r="H35" s="11">
         <v>42402</v>
       </c>
       <c r="I35" s="3" t="s">
@@ -2050,7 +2050,7 @@
       <c r="G36" t="s">
         <v>23</v>
       </c>
-      <c r="H36" s="13">
+      <c r="H36" s="11">
         <v>41116</v>
       </c>
       <c r="I36" s="3" t="s">
@@ -2108,7 +2108,7 @@
       <c r="G38" t="s">
         <v>31</v>
       </c>
-      <c r="H38" s="14">
+      <c r="H38" s="12">
         <v>39681</v>
       </c>
       <c r="I38" s="3" t="s">
@@ -2138,7 +2138,7 @@
       <c r="G39" t="s">
         <v>78</v>
       </c>
-      <c r="H39" s="11">
+      <c r="H39" s="9">
         <v>39904</v>
       </c>
       <c r="I39" s="3" t="s">
@@ -2224,7 +2224,7 @@
       <c r="G42" t="s">
         <v>78</v>
       </c>
-      <c r="H42" s="13">
+      <c r="H42" s="11">
         <v>41944</v>
       </c>
       <c r="I42" s="8" t="s">
@@ -2256,7 +2256,7 @@
       <c r="G43" t="s">
         <v>89</v>
       </c>
-      <c r="H43" s="11">
+      <c r="H43" s="9">
         <v>39791</v>
       </c>
       <c r="I43" s="3" t="s">
@@ -2286,7 +2286,7 @@
       <c r="G44" t="s">
         <v>91</v>
       </c>
-      <c r="H44" s="15"/>
+      <c r="H44" s="13"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8"/>
     </row>
@@ -2312,7 +2312,7 @@
       <c r="G45" t="s">
         <v>42</v>
       </c>
-      <c r="H45" s="13">
+      <c r="H45" s="11">
         <v>39234</v>
       </c>
       <c r="I45" s="3" t="s">
@@ -2370,7 +2370,7 @@
       <c r="G47" t="s">
         <v>95</v>
       </c>
-      <c r="H47" s="15"/>
+      <c r="H47" s="13"/>
       <c r="I47" s="8"/>
       <c r="J47" s="8"/>
     </row>
@@ -2396,7 +2396,7 @@
       <c r="G48" t="s">
         <v>23</v>
       </c>
-      <c r="H48" s="13">
+      <c r="H48" s="11">
         <v>41071</v>
       </c>
       <c r="I48" s="3" t="s">
@@ -2452,7 +2452,7 @@
       <c r="G50" t="s">
         <v>23</v>
       </c>
-      <c r="H50" s="13">
+      <c r="H50" s="11">
         <v>40544</v>
       </c>
       <c r="I50" s="2" t="s">
@@ -2482,7 +2482,7 @@
       <c r="G51" t="s">
         <v>78</v>
       </c>
-      <c r="H51" s="13">
+      <c r="H51" s="11">
         <v>41395</v>
       </c>
       <c r="I51" s="3" t="s">
@@ -2538,7 +2538,7 @@
       <c r="G53" t="s">
         <v>78</v>
       </c>
-      <c r="H53" s="13">
+      <c r="H53" s="11">
         <v>41913</v>
       </c>
       <c r="I53" s="3" t="s">
@@ -2648,7 +2648,7 @@
       <c r="G57" t="s">
         <v>42</v>
       </c>
-      <c r="H57" s="13">
+      <c r="H57" s="11">
         <v>40848</v>
       </c>
       <c r="I57" s="3" t="s">
@@ -2678,7 +2678,7 @@
       <c r="G58" t="s">
         <v>109</v>
       </c>
-      <c r="H58" s="13">
+      <c r="H58" s="11">
         <v>40837</v>
       </c>
       <c r="I58" s="3" t="s">
@@ -2708,7 +2708,7 @@
       <c r="G59" t="s">
         <v>69</v>
       </c>
-      <c r="H59" s="13">
+      <c r="H59" s="11">
         <v>41214</v>
       </c>
       <c r="I59" s="3" t="s">
@@ -2921,15 +2921,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
       <c r="I1" s="3" t="s">
         <v>137</v>
       </c>
@@ -2985,7 +2985,7 @@
       <c r="G3" s="5">
         <v>42401</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="9">
         <v>42297</v>
       </c>
       <c r="I3" s="3" t="s">
@@ -3022,28 +3022,28 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="16">
+      <c r="D5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="14">
         <v>42826</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="14">
         <v>42826</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="14">
         <v>42826</v>
       </c>
-      <c r="H5" s="15"/>
+      <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="8" t="s">
@@ -3067,7 +3067,7 @@
       <c r="G6" s="5">
         <v>40179</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <v>39161</v>
       </c>
       <c r="I6" s="3" t="s">
@@ -3131,7 +3131,7 @@
       <c r="G8" s="5">
         <v>40725</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="10">
         <v>38930</v>
       </c>
       <c r="I8" s="3" t="s">
@@ -3160,7 +3160,7 @@
       <c r="G9" s="5">
         <v>42309</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="12">
         <v>42010</v>
       </c>
       <c r="I9" s="3" t="s">
@@ -3189,7 +3189,7 @@
       <c r="G10" s="5">
         <v>41183</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="11">
         <v>40459</v>
       </c>
       <c r="I10" s="2" t="s">
@@ -3241,7 +3241,7 @@
       <c r="G12" s="5">
         <v>41183</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="9">
         <v>41192</v>
       </c>
       <c r="I12" s="3" t="s">
@@ -3270,7 +3270,7 @@
       <c r="G13" s="5">
         <v>42522</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="11">
         <v>42461</v>
       </c>
       <c r="I13" s="2" t="s">
@@ -3322,7 +3322,7 @@
       <c r="G15" s="5">
         <v>41275</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="10">
         <v>38777</v>
       </c>
       <c r="I15" s="3" t="s">
@@ -3351,7 +3351,7 @@
       <c r="G16" s="5">
         <v>41821</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="12">
         <v>40856</v>
       </c>
       <c r="I16" s="3" t="s">
@@ -3380,7 +3380,7 @@
       <c r="G17" s="5">
         <v>41275</v>
       </c>
-      <c r="H17" s="13">
+      <c r="H17" s="11">
         <v>40664</v>
       </c>
       <c r="I17" s="2" t="s">
@@ -3409,7 +3409,7 @@
       <c r="G18" s="5">
         <v>40179</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="10">
         <v>39264</v>
       </c>
       <c r="I18" s="3" t="s">
@@ -3438,7 +3438,7 @@
       <c r="G19" s="5">
         <v>41275</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="11">
         <v>38758</v>
       </c>
       <c r="I19" s="3" t="s">
@@ -3467,7 +3467,7 @@
       <c r="G20" s="5">
         <v>41275</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="11">
         <v>40848</v>
       </c>
       <c r="I20" s="3" t="s">
@@ -3652,7 +3652,7 @@
       <c r="G27" s="5">
         <v>41821</v>
       </c>
-      <c r="H27" s="13">
+      <c r="H27" s="11">
         <v>41153</v>
       </c>
       <c r="I27" s="3" t="s">
@@ -3684,7 +3684,7 @@
       <c r="G28" s="5">
         <v>40603</v>
       </c>
-      <c r="H28" s="12">
+      <c r="H28" s="10">
         <v>40165</v>
       </c>
       <c r="I28" s="3" t="s">
@@ -3716,7 +3716,7 @@
       <c r="G29" s="5">
         <v>41610</v>
       </c>
-      <c r="H29" s="13">
+      <c r="H29" s="11">
         <v>40695</v>
       </c>
       <c r="I29" s="3" t="s">
@@ -3727,28 +3727,28 @@
       </c>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" s="16">
+      <c r="D30" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="14">
         <v>43131</v>
       </c>
-      <c r="F30" s="16">
+      <c r="F30" s="14">
         <v>43131</v>
       </c>
-      <c r="G30" s="16">
+      <c r="G30" s="14">
         <v>43131</v>
       </c>
-      <c r="H30" s="15"/>
+      <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="8" t="s">
@@ -3772,7 +3772,7 @@
       <c r="G31" s="5">
         <v>41275</v>
       </c>
-      <c r="H31" s="13">
+      <c r="H31" s="11">
         <v>41183</v>
       </c>
       <c r="I31" s="3" t="s">
@@ -3801,7 +3801,7 @@
       <c r="G32" s="5">
         <v>41275</v>
       </c>
-      <c r="H32" s="13">
+      <c r="H32" s="11">
         <v>40645</v>
       </c>
       <c r="I32" s="2" t="s">
@@ -3833,7 +3833,7 @@
       <c r="G33" s="5">
         <v>41306</v>
       </c>
-      <c r="H33" s="13">
+      <c r="H33" s="11">
         <v>40264</v>
       </c>
       <c r="I33" s="3" t="s">
@@ -3888,7 +3888,7 @@
       <c r="G35" s="5">
         <v>42461</v>
       </c>
-      <c r="H35" s="13">
+      <c r="H35" s="11">
         <v>42402</v>
       </c>
       <c r="I35" s="3" t="s">
@@ -3917,7 +3917,7 @@
       <c r="G36" s="5">
         <v>41821</v>
       </c>
-      <c r="H36" s="13">
+      <c r="H36" s="11">
         <v>41116</v>
       </c>
       <c r="I36" s="3" t="s">
@@ -3972,7 +3972,7 @@
       <c r="G38" s="5">
         <v>41183</v>
       </c>
-      <c r="H38" s="14">
+      <c r="H38" s="12">
         <v>39681</v>
       </c>
       <c r="I38" s="3" t="s">
@@ -4002,7 +4002,7 @@
       <c r="G39" s="5">
         <v>42005</v>
       </c>
-      <c r="H39" s="11">
+      <c r="H39" s="9">
         <v>39904</v>
       </c>
       <c r="I39" s="3" t="s">
@@ -4083,7 +4083,7 @@
       <c r="G42" s="5">
         <v>42005</v>
       </c>
-      <c r="H42" s="13">
+      <c r="H42" s="11">
         <v>41944</v>
       </c>
       <c r="I42" s="8" t="s">
@@ -4115,7 +4115,7 @@
       <c r="G43" s="5">
         <v>40911</v>
       </c>
-      <c r="H43" s="11">
+      <c r="H43" s="9">
         <v>39791</v>
       </c>
       <c r="I43" s="3" t="s">
@@ -4123,28 +4123,28 @@
       </c>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C44" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D44" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E44" s="16">
+      <c r="D44" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="14">
         <v>43009</v>
       </c>
-      <c r="F44" s="16">
+      <c r="F44" s="14">
         <v>43009</v>
       </c>
-      <c r="G44" s="16">
+      <c r="G44" s="14">
         <v>43009</v>
       </c>
-      <c r="H44" s="15"/>
+      <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="8" t="s">
@@ -4168,7 +4168,7 @@
       <c r="G45" s="5">
         <v>41275</v>
       </c>
-      <c r="H45" s="13">
+      <c r="H45" s="11">
         <v>39234</v>
       </c>
       <c r="I45" s="3" t="s">
@@ -4202,28 +4202,28 @@
       </c>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="C47" s="15" t="s">
+      <c r="C47" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="D47" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E47" s="16">
+      <c r="D47" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="14">
         <v>43115</v>
       </c>
-      <c r="F47" s="16">
+      <c r="F47" s="14">
         <v>43115</v>
       </c>
-      <c r="G47" s="16">
+      <c r="G47" s="14">
         <v>43115</v>
       </c>
-      <c r="H47" s="15"/>
+      <c r="H47" s="13"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="8" t="s">
@@ -4247,7 +4247,7 @@
       <c r="G48" s="5">
         <v>41821</v>
       </c>
-      <c r="H48" s="13">
+      <c r="H48" s="11">
         <v>41071</v>
       </c>
       <c r="I48" s="3" t="s">
@@ -4299,7 +4299,7 @@
       <c r="G50" s="5">
         <v>41821</v>
       </c>
-      <c r="H50" s="13">
+      <c r="H50" s="11">
         <v>40544</v>
       </c>
       <c r="I50" s="2" t="s">
@@ -4328,7 +4328,7 @@
       <c r="G51" s="5">
         <v>42005</v>
       </c>
-      <c r="H51" s="13">
+      <c r="H51" s="11">
         <v>41395</v>
       </c>
       <c r="I51" s="3" t="s">
@@ -4380,7 +4380,7 @@
       <c r="G53" s="5">
         <v>42005</v>
       </c>
-      <c r="H53" s="13">
+      <c r="H53" s="11">
         <v>41913</v>
       </c>
       <c r="I53" s="3" t="s">
@@ -4481,7 +4481,7 @@
       <c r="G57" s="5">
         <v>41275</v>
       </c>
-      <c r="H57" s="13">
+      <c r="H57" s="11">
         <v>40848</v>
       </c>
       <c r="I57" s="3" t="s">
@@ -4510,7 +4510,7 @@
       <c r="G58" s="5">
         <v>41366</v>
       </c>
-      <c r="H58" s="13">
+      <c r="H58" s="11">
         <v>40837</v>
       </c>
       <c r="I58" s="3" t="s">
@@ -4539,7 +4539,7 @@
       <c r="G59" s="5">
         <v>41306</v>
       </c>
-      <c r="H59" s="13">
+      <c r="H59" s="11">
         <v>41214</v>
       </c>
       <c r="I59" s="3" t="s">

</xml_diff>